<commit_message>
Create V0.4 Logic Board KiCad Project
</commit_message>
<xml_diff>
--- a/Manufacturing/BOM Core 64 v0.4.0 Yellow Dual Boards.xlsx
+++ b/Manufacturing/BOM Core 64 v0.4.0 Yellow Dual Boards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ageppert/Dropbox/Electronics/Core 64 Interactive Badge/Core-64-Interactive-Core-Memory-Badge/Manufacturing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD7E5BCC-D09C-FC42-A3E5-B95A446E99E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA52FDED-C001-D54E-8FB0-4B2F6ADEF0B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13960" yWindow="460" windowWidth="35600" windowHeight="27080" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="925" uniqueCount="529">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="932" uniqueCount="538">
   <si>
     <t>Digi-Key Part Number</t>
   </si>
@@ -1647,6 +1647,33 @@
   <si>
     <t>Sparkfun DEV-13736</t>
   </si>
+  <si>
+    <t>Labor: Test</t>
+  </si>
+  <si>
+    <t>Labor: Set EEPROM S/N, print sticker, attach sticker</t>
+  </si>
+  <si>
+    <t>Labor: Assembly</t>
+  </si>
+  <si>
+    <t>Labor: Package</t>
+  </si>
+  <si>
+    <t>Final Package Box</t>
+  </si>
+  <si>
+    <t>Product Labels</t>
+  </si>
+  <si>
+    <t>Instruction Manual</t>
+  </si>
+  <si>
+    <t>ESD Bag for Logic Board</t>
+  </si>
+  <si>
+    <t>ESD Bag for Teensy 3.2 and Headers</t>
+  </si>
 </sst>
 </file>
 
@@ -1657,10 +1684,17 @@
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.000_);_(&quot;$&quot;* \(#,##0.000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1878,36 +1912,36 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="13" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="12" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="11" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1917,172 +1951,84 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="9" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="10" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="10" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="10" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="14" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="15" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="6" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -2090,26 +2036,120 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="10" fillId="6" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -4909,11 +4949,11 @@
         <v>173</v>
       </c>
       <c r="C3" s="27"/>
-      <c r="P3" s="66" t="s">
+      <c r="P3" s="91" t="s">
         <v>174</v>
       </c>
-      <c r="Q3" s="66"/>
-      <c r="R3" s="66"/>
+      <c r="Q3" s="91"/>
+      <c r="R3" s="91"/>
     </row>
     <row r="4" spans="1:18" ht="51" x14ac:dyDescent="0.15">
       <c r="A4" s="29"/>
@@ -4972,7 +5012,7 @@
       <c r="B6" s="39" t="s">
         <v>189</v>
       </c>
-      <c r="C6" s="68" t="s">
+      <c r="C6" s="67" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="39" t="s">
@@ -5019,7 +5059,7 @@
       </c>
     </row>
     <row r="7" spans="1:18" s="39" customFormat="1" ht="24" x14ac:dyDescent="0.15">
-      <c r="A7" s="69" t="s">
+      <c r="A7" s="68" t="s">
         <v>487</v>
       </c>
       <c r="R7" s="40"/>
@@ -5031,10 +5071,10 @@
       <c r="B8" s="55" t="s">
         <v>142</v>
       </c>
-      <c r="C8" s="67" t="s">
+      <c r="C8" s="66" t="s">
         <v>488</v>
       </c>
-      <c r="D8" s="67" t="s">
+      <c r="D8" s="66" t="s">
         <v>483</v>
       </c>
       <c r="E8" s="55">
@@ -5176,7 +5216,7 @@
       <c r="B11" s="56" t="s">
         <v>223</v>
       </c>
-      <c r="C11" s="67" t="s">
+      <c r="C11" s="66" t="s">
         <v>490</v>
       </c>
       <c r="D11" s="55" t="s">
@@ -5224,7 +5264,7 @@
       <c r="B12" s="56" t="s">
         <v>364</v>
       </c>
-      <c r="C12" s="67" t="s">
+      <c r="C12" s="66" t="s">
         <v>490</v>
       </c>
       <c r="D12" s="55" t="s">
@@ -5272,7 +5312,7 @@
       <c r="B13" s="56" t="s">
         <v>224</v>
       </c>
-      <c r="C13" s="67" t="s">
+      <c r="C13" s="66" t="s">
         <v>490</v>
       </c>
       <c r="D13" s="55" t="s">
@@ -5320,7 +5360,7 @@
       <c r="B14" s="56" t="s">
         <v>372</v>
       </c>
-      <c r="C14" s="67" t="s">
+      <c r="C14" s="66" t="s">
         <v>490</v>
       </c>
       <c r="D14" s="55" t="s">
@@ -5368,7 +5408,7 @@
       <c r="B15" s="56" t="s">
         <v>225</v>
       </c>
-      <c r="C15" s="67" t="s">
+      <c r="C15" s="66" t="s">
         <v>491</v>
       </c>
       <c r="D15" s="61" t="s">
@@ -5410,14 +5450,14 @@
       </c>
     </row>
     <row r="16" spans="1:18" s="39" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="68" t="s">
+      <c r="B16" s="67" t="s">
         <v>509</v>
       </c>
-      <c r="C16" s="68"/>
-      <c r="D16" s="70"/>
-      <c r="G16" s="70"/>
-      <c r="H16" s="71"/>
-      <c r="I16" s="71"/>
+      <c r="C16" s="67"/>
+      <c r="D16" s="69"/>
+      <c r="G16" s="69"/>
+      <c r="H16" s="70"/>
+      <c r="I16" s="70"/>
       <c r="R16" s="40"/>
     </row>
     <row r="17" spans="1:18" s="35" customFormat="1" x14ac:dyDescent="0.2">
@@ -5508,7 +5548,7 @@
       <c r="R19" s="28"/>
     </row>
     <row r="20" spans="1:18" s="35" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="73" t="s">
+      <c r="B20" s="72" t="s">
         <v>506</v>
       </c>
       <c r="C20" s="52"/>
@@ -5521,7 +5561,7 @@
       <c r="R20" s="28"/>
     </row>
     <row r="21" spans="1:18" s="35" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="73" t="s">
+      <c r="B21" s="72" t="s">
         <v>507</v>
       </c>
       <c r="C21" s="52"/>
@@ -5534,7 +5574,7 @@
       <c r="R21" s="28"/>
     </row>
     <row r="22" spans="1:18" s="35" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="73"/>
+      <c r="B22" s="72"/>
       <c r="C22" s="52"/>
       <c r="D22" s="36"/>
       <c r="F22" s="28"/>
@@ -5545,7 +5585,7 @@
       <c r="R22" s="28"/>
     </row>
     <row r="23" spans="1:18" s="39" customFormat="1" ht="24" x14ac:dyDescent="0.15">
-      <c r="A23" s="69" t="s">
+      <c r="A23" s="68" t="s">
         <v>484</v>
       </c>
       <c r="R23" s="40"/>
@@ -5554,10 +5594,10 @@
       <c r="A24" s="54" t="s">
         <v>456</v>
       </c>
-      <c r="B24" s="67" t="s">
+      <c r="B24" s="66" t="s">
         <v>486</v>
       </c>
-      <c r="C24" s="67" t="s">
+      <c r="C24" s="66" t="s">
         <v>496</v>
       </c>
       <c r="D24" s="56" t="s">
@@ -5600,7 +5640,7 @@
       <c r="B25" s="55" t="s">
         <v>218</v>
       </c>
-      <c r="C25" s="67" t="s">
+      <c r="C25" s="66" t="s">
         <v>492</v>
       </c>
       <c r="D25" s="61" t="s">
@@ -5648,7 +5688,7 @@
       <c r="B26" s="55" t="s">
         <v>218</v>
       </c>
-      <c r="C26" s="67" t="s">
+      <c r="C26" s="66" t="s">
         <v>493</v>
       </c>
       <c r="D26" s="56" t="s">
@@ -5693,7 +5733,7 @@
       <c r="B27" s="55" t="s">
         <v>218</v>
       </c>
-      <c r="C27" s="67" t="s">
+      <c r="C27" s="66" t="s">
         <v>493</v>
       </c>
       <c r="D27" s="61" t="s">
@@ -5722,11 +5762,11 @@
         <v>4</v>
       </c>
       <c r="M27" s="28">
-        <f>L27-E27</f>
+        <f t="shared" ref="M27:M32" si="10">L27-E27</f>
         <v>-4</v>
       </c>
       <c r="N27" s="28">
-        <f>(4*E27)-M27</f>
+        <f t="shared" ref="N27:N32" si="11">(4*E27)-M27</f>
         <v>20</v>
       </c>
       <c r="R27" s="32"/>
@@ -5738,7 +5778,7 @@
       <c r="B28" s="55" t="s">
         <v>232</v>
       </c>
-      <c r="C28" s="67" t="s">
+      <c r="C28" s="66" t="s">
         <v>494</v>
       </c>
       <c r="D28" s="61" t="s">
@@ -5767,11 +5807,11 @@
         <v>0</v>
       </c>
       <c r="M28" s="28">
-        <f>L28-E28</f>
+        <f t="shared" si="10"/>
         <v>-1</v>
       </c>
       <c r="N28" s="28">
-        <f>(4*E28)-M28</f>
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
       <c r="R28" s="32" t="e">
@@ -5819,11 +5859,11 @@
         <v>860</v>
       </c>
       <c r="M29" s="28">
-        <f>L29-E29</f>
+        <f t="shared" si="10"/>
         <v>790</v>
       </c>
       <c r="N29" s="28">
-        <f>(4*E29)-M29</f>
+        <f t="shared" si="11"/>
         <v>-510</v>
       </c>
       <c r="R29" s="32" t="e">
@@ -5871,11 +5911,11 @@
         <v>426.2</v>
       </c>
       <c r="M30" s="28">
-        <f>L30-E30</f>
+        <f t="shared" si="10"/>
         <v>425.4</v>
       </c>
       <c r="N30" s="28">
-        <f>(4*E30)-M30</f>
+        <f t="shared" si="11"/>
         <v>-422.2</v>
       </c>
       <c r="P30" s="28">
@@ -5925,11 +5965,11 @@
         <v>100</v>
       </c>
       <c r="M31" s="28">
-        <f>L31-E31</f>
+        <f t="shared" si="10"/>
         <v>99.2</v>
       </c>
       <c r="N31" s="28">
-        <f>(4*E31)-M31</f>
+        <f t="shared" si="11"/>
         <v>-96</v>
       </c>
       <c r="P31" s="28">
@@ -5982,11 +6022,11 @@
         <v>747</v>
       </c>
       <c r="M32" s="33">
-        <f>L32-E32</f>
+        <f t="shared" si="10"/>
         <v>746.25</v>
       </c>
       <c r="N32" s="33">
-        <f>(4*E32)-M32</f>
+        <f t="shared" si="11"/>
         <v>-743.25</v>
       </c>
       <c r="P32" s="28">
@@ -6002,7 +6042,7 @@
       </c>
     </row>
     <row r="33" spans="1:18" s="39" customFormat="1" ht="17" x14ac:dyDescent="0.15">
-      <c r="B33" s="68" t="s">
+      <c r="B33" s="67" t="s">
         <v>167</v>
       </c>
       <c r="J33" s="41"/>
@@ -6014,7 +6054,7 @@
       <c r="R33" s="40"/>
     </row>
     <row r="34" spans="1:18" s="39" customFormat="1" ht="17" x14ac:dyDescent="0.15">
-      <c r="B34" s="68" t="s">
+      <c r="B34" s="67" t="s">
         <v>510</v>
       </c>
       <c r="J34" s="41"/>
@@ -6026,13 +6066,13 @@
       <c r="R34" s="40"/>
     </row>
     <row r="35" spans="1:18" s="39" customFormat="1" ht="24" x14ac:dyDescent="0.15">
-      <c r="A35" s="69" t="s">
+      <c r="A35" s="68" t="s">
         <v>485</v>
       </c>
-      <c r="D35" s="70"/>
-      <c r="G35" s="71"/>
-      <c r="H35" s="71"/>
-      <c r="I35" s="70"/>
+      <c r="D35" s="69"/>
+      <c r="G35" s="70"/>
+      <c r="H35" s="70"/>
+      <c r="I35" s="69"/>
       <c r="R35" s="40"/>
     </row>
     <row r="36" spans="1:18" ht="34" x14ac:dyDescent="0.15">
@@ -6042,7 +6082,7 @@
       <c r="B36" s="56" t="s">
         <v>451</v>
       </c>
-      <c r="C36" s="67" t="s">
+      <c r="C36" s="66" t="s">
         <v>495</v>
       </c>
       <c r="D36" s="61" t="s">
@@ -6090,7 +6130,7 @@
       <c r="B37" s="58" t="s">
         <v>454</v>
       </c>
-      <c r="C37" s="67" t="s">
+      <c r="C37" s="66" t="s">
         <v>495</v>
       </c>
       <c r="D37" s="61" t="s">
@@ -6120,15 +6160,15 @@
       </c>
       <c r="L37" s="39"/>
       <c r="M37" s="28">
-        <f t="shared" ref="M37" si="10">L37-E37</f>
+        <f t="shared" ref="M37" si="12">L37-E37</f>
         <v>-2</v>
       </c>
       <c r="N37" s="28">
-        <f t="shared" ref="N37" si="11">(4*E37)-M37</f>
+        <f t="shared" ref="N37" si="13">(4*E37)-M37</f>
         <v>10</v>
       </c>
       <c r="R37" s="32" t="e">
-        <f t="shared" ref="R37" si="12">Q37/P37</f>
+        <f t="shared" ref="R37" si="14">Q37/P37</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -6147,10 +6187,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1052A41E-3EA7-B148-953B-E2218E71D84C}">
-  <dimension ref="A1:AE82"/>
+  <dimension ref="A1:AE86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="125" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D84" sqref="D84"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="125" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.15"/>
@@ -6218,11 +6258,11 @@
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.15">
-      <c r="P7" s="66" t="s">
+      <c r="P7" s="91" t="s">
         <v>174</v>
       </c>
-      <c r="Q7" s="66"/>
-      <c r="R7" s="66"/>
+      <c r="Q7" s="91"/>
+      <c r="R7" s="91"/>
     </row>
     <row r="8" spans="1:31" ht="17" x14ac:dyDescent="0.15">
       <c r="A8" s="27" t="s">
@@ -6289,13 +6329,13 @@
       <c r="B10" s="28" t="s">
         <v>189</v>
       </c>
-      <c r="C10" s="72" t="s">
+      <c r="C10" s="71" t="s">
         <v>3</v>
       </c>
       <c r="D10" s="27" t="s">
         <v>246</v>
       </c>
-      <c r="E10" s="75" t="s">
+      <c r="E10" s="74" t="s">
         <v>247</v>
       </c>
       <c r="F10" s="28" t="s">
@@ -6386,7 +6426,7 @@
       <c r="D11" s="27" t="s">
         <v>262</v>
       </c>
-      <c r="E11" s="75">
+      <c r="E11" s="74">
         <v>2</v>
       </c>
       <c r="F11" s="28" t="s">
@@ -6443,7 +6483,7 @@
       <c r="D12" s="27" t="s">
         <v>268</v>
       </c>
-      <c r="E12" s="75">
+      <c r="E12" s="74">
         <v>7</v>
       </c>
       <c r="F12" s="28" t="s">
@@ -6500,7 +6540,7 @@
       <c r="D13" s="27" t="s">
         <v>268</v>
       </c>
-      <c r="E13" s="75">
+      <c r="E13" s="74">
         <v>2</v>
       </c>
       <c r="F13" s="28" t="s">
@@ -6553,19 +6593,19 @@
         <v>272</v>
       </c>
       <c r="C14" s="30"/>
-      <c r="D14" s="76" t="s">
+      <c r="D14" s="75" t="s">
         <v>273</v>
       </c>
-      <c r="E14" s="77">
+      <c r="E14" s="76">
         <v>1</v>
       </c>
       <c r="F14" s="30" t="s">
         <v>201</v>
       </c>
-      <c r="G14" s="78" t="s">
+      <c r="G14" s="77" t="s">
         <v>438</v>
       </c>
-      <c r="H14" s="79" t="s">
+      <c r="H14" s="78" t="s">
         <v>274</v>
       </c>
       <c r="I14" s="27" t="s">
@@ -6616,7 +6656,7 @@
       <c r="D15" s="27" t="s">
         <v>278</v>
       </c>
-      <c r="E15" s="75">
+      <c r="E15" s="74">
         <v>6</v>
       </c>
       <c r="F15" s="28" t="s">
@@ -6677,7 +6717,7 @@
       <c r="D16" s="27" t="s">
         <v>278</v>
       </c>
-      <c r="E16" s="75">
+      <c r="E16" s="74">
         <v>6</v>
       </c>
       <c r="F16" s="28" t="s">
@@ -6735,16 +6775,16 @@
         <v>285</v>
       </c>
       <c r="C17" s="30"/>
-      <c r="D17" s="76" t="s">
+      <c r="D17" s="75" t="s">
         <v>286</v>
       </c>
-      <c r="E17" s="77">
+      <c r="E17" s="76">
         <v>1</v>
       </c>
       <c r="F17" s="30" t="s">
         <v>201</v>
       </c>
-      <c r="G17" s="76" t="s">
+      <c r="G17" s="75" t="s">
         <v>287</v>
       </c>
       <c r="H17" s="27" t="s">
@@ -6791,7 +6831,7 @@
       <c r="B18" s="28"/>
       <c r="C18" s="28"/>
       <c r="D18" s="27"/>
-      <c r="E18" s="75"/>
+      <c r="E18" s="74"/>
       <c r="G18" s="27"/>
       <c r="H18" s="27"/>
       <c r="K18" s="28"/>
@@ -6814,7 +6854,7 @@
       <c r="B19" s="28"/>
       <c r="C19" s="28"/>
       <c r="D19" s="27"/>
-      <c r="E19" s="75"/>
+      <c r="E19" s="74"/>
       <c r="G19" s="27"/>
       <c r="H19" s="27"/>
       <c r="K19" s="28"/>
@@ -6838,19 +6878,19 @@
         <v>289</v>
       </c>
       <c r="C20" s="30"/>
-      <c r="D20" s="76" t="s">
+      <c r="D20" s="75" t="s">
         <v>290</v>
       </c>
-      <c r="E20" s="77">
+      <c r="E20" s="76">
         <v>1</v>
       </c>
       <c r="F20" s="30" t="s">
         <v>201</v>
       </c>
-      <c r="G20" s="79" t="s">
+      <c r="G20" s="78" t="s">
         <v>291</v>
       </c>
-      <c r="H20" s="79" t="s">
+      <c r="H20" s="78" t="s">
         <v>292</v>
       </c>
       <c r="I20" s="27" t="s">
@@ -6907,19 +6947,19 @@
         <v>298</v>
       </c>
       <c r="C21" s="38"/>
-      <c r="D21" s="80" t="s">
+      <c r="D21" s="79" t="s">
         <v>299</v>
       </c>
-      <c r="E21" s="81">
+      <c r="E21" s="80">
         <v>1</v>
       </c>
       <c r="F21" s="38" t="s">
         <v>201</v>
       </c>
-      <c r="G21" s="80" t="s">
+      <c r="G21" s="79" t="s">
         <v>300</v>
       </c>
-      <c r="H21" s="80" t="s">
+      <c r="H21" s="79" t="s">
         <v>301</v>
       </c>
       <c r="I21" s="27" t="s">
@@ -6967,7 +7007,7 @@
       <c r="D22" s="27" t="s">
         <v>304</v>
       </c>
-      <c r="E22" s="75">
+      <c r="E22" s="74">
         <v>4</v>
       </c>
       <c r="F22" s="28" t="s">
@@ -7024,16 +7064,16 @@
       <c r="D23" s="27" t="s">
         <v>309</v>
       </c>
-      <c r="E23" s="75">
+      <c r="E23" s="74">
         <v>1</v>
       </c>
       <c r="F23" s="28" t="s">
         <v>201</v>
       </c>
-      <c r="G23" s="82" t="s">
+      <c r="G23" s="81" t="s">
         <v>310</v>
       </c>
-      <c r="H23" s="72" t="s">
+      <c r="H23" s="71" t="s">
         <v>311</v>
       </c>
       <c r="I23" s="27" t="s">
@@ -7081,7 +7121,7 @@
       <c r="D24" s="27" t="s">
         <v>314</v>
       </c>
-      <c r="E24" s="75">
+      <c r="E24" s="74">
         <v>2</v>
       </c>
       <c r="F24" s="28" t="s">
@@ -7134,7 +7174,7 @@
       <c r="B25" s="28"/>
       <c r="C25" s="28"/>
       <c r="D25" s="27"/>
-      <c r="E25" s="75"/>
+      <c r="E25" s="74"/>
       <c r="G25" s="27"/>
       <c r="H25" s="27"/>
       <c r="K25" s="28"/>
@@ -7154,7 +7194,7 @@
       <c r="B26" s="28"/>
       <c r="C26" s="28"/>
       <c r="D26" s="27"/>
-      <c r="E26" s="75"/>
+      <c r="E26" s="74"/>
       <c r="G26" s="27"/>
       <c r="H26" s="27"/>
       <c r="K26" s="28"/>
@@ -7174,7 +7214,7 @@
       <c r="B27" s="28"/>
       <c r="C27" s="28"/>
       <c r="D27" s="27"/>
-      <c r="E27" s="75"/>
+      <c r="E27" s="74"/>
       <c r="G27" s="27"/>
       <c r="H27" s="27"/>
       <c r="K27" s="28"/>
@@ -7194,7 +7234,7 @@
       <c r="B28" s="28"/>
       <c r="C28" s="28"/>
       <c r="D28" s="27"/>
-      <c r="E28" s="75"/>
+      <c r="E28" s="74"/>
       <c r="G28" s="27"/>
       <c r="H28" s="27"/>
       <c r="K28" s="28"/>
@@ -7214,7 +7254,7 @@
       <c r="B29" s="28"/>
       <c r="C29" s="28"/>
       <c r="D29" s="27"/>
-      <c r="E29" s="75"/>
+      <c r="E29" s="74"/>
       <c r="G29" s="27"/>
       <c r="H29" s="27"/>
       <c r="K29" s="28"/>
@@ -7230,7 +7270,7 @@
       <c r="B30" s="28"/>
       <c r="C30" s="28"/>
       <c r="D30" s="27"/>
-      <c r="E30" s="75"/>
+      <c r="E30" s="74"/>
       <c r="G30" s="27"/>
       <c r="H30" s="27"/>
       <c r="K30" s="28"/>
@@ -7247,16 +7287,16 @@
         <v>318</v>
       </c>
       <c r="C31" s="30"/>
-      <c r="D31" s="76" t="s">
+      <c r="D31" s="75" t="s">
         <v>319</v>
       </c>
-      <c r="E31" s="77">
+      <c r="E31" s="76">
         <v>1</v>
       </c>
       <c r="F31" s="30" t="s">
         <v>201</v>
       </c>
-      <c r="G31" s="76" t="s">
+      <c r="G31" s="75" t="s">
         <v>320</v>
       </c>
       <c r="H31" s="27" t="s">
@@ -7303,7 +7343,7 @@
       <c r="D32" s="27" t="s">
         <v>319</v>
       </c>
-      <c r="E32" s="75">
+      <c r="E32" s="74">
         <v>10</v>
       </c>
       <c r="F32" s="28" t="s">
@@ -7379,7 +7419,7 @@
       <c r="D33" s="27" t="s">
         <v>319</v>
       </c>
-      <c r="E33" s="75">
+      <c r="E33" s="74">
         <v>11</v>
       </c>
       <c r="F33" s="28" t="s">
@@ -7452,16 +7492,16 @@
         <v>336</v>
       </c>
       <c r="C34" s="30"/>
-      <c r="D34" s="76" t="s">
+      <c r="D34" s="75" t="s">
         <v>337</v>
       </c>
-      <c r="E34" s="77">
+      <c r="E34" s="76">
         <v>1</v>
       </c>
       <c r="F34" s="30" t="s">
         <v>201</v>
       </c>
-      <c r="G34" s="76">
+      <c r="G34" s="75">
         <v>0.1</v>
       </c>
       <c r="H34" s="27"/>
@@ -7503,16 +7543,16 @@
         <v>339</v>
       </c>
       <c r="C35" s="30"/>
-      <c r="D35" s="76" t="s">
+      <c r="D35" s="75" t="s">
         <v>337</v>
       </c>
-      <c r="E35" s="77">
+      <c r="E35" s="76">
         <v>2</v>
       </c>
       <c r="F35" s="30" t="s">
         <v>201</v>
       </c>
-      <c r="G35" s="76" t="s">
+      <c r="G35" s="75" t="s">
         <v>222</v>
       </c>
       <c r="H35" s="27" t="s">
@@ -7558,7 +7598,7 @@
       <c r="D36" s="27" t="s">
         <v>337</v>
       </c>
-      <c r="E36" s="75">
+      <c r="E36" s="74">
         <v>1</v>
       </c>
       <c r="F36" s="28" t="s">
@@ -7567,7 +7607,7 @@
       <c r="G36" s="27">
         <v>300</v>
       </c>
-      <c r="H36" s="80" t="s">
+      <c r="H36" s="79" t="s">
         <v>341</v>
       </c>
       <c r="I36" s="27" t="s">
@@ -7608,7 +7648,7 @@
       <c r="D37" s="27" t="s">
         <v>337</v>
       </c>
-      <c r="E37" s="75">
+      <c r="E37" s="74">
         <v>21</v>
       </c>
       <c r="F37" s="28" t="s">
@@ -7660,7 +7700,7 @@
       <c r="D38" s="27" t="s">
         <v>337</v>
       </c>
-      <c r="E38" s="75">
+      <c r="E38" s="74">
         <v>6</v>
       </c>
       <c r="F38" s="28" t="s">
@@ -7712,7 +7752,7 @@
       <c r="D39" s="27" t="s">
         <v>337</v>
       </c>
-      <c r="E39" s="75">
+      <c r="E39" s="74">
         <v>3</v>
       </c>
       <c r="F39" s="28" t="s">
@@ -7765,7 +7805,7 @@
       <c r="D40" s="27" t="s">
         <v>337</v>
       </c>
-      <c r="E40" s="75">
+      <c r="E40" s="74">
         <v>2</v>
       </c>
       <c r="F40" s="28" t="s">
@@ -7818,7 +7858,7 @@
       <c r="D41" s="27" t="s">
         <v>337</v>
       </c>
-      <c r="E41" s="75">
+      <c r="E41" s="74">
         <v>2</v>
       </c>
       <c r="F41" s="28" t="s">
@@ -7870,7 +7910,7 @@
       <c r="D42" s="27" t="s">
         <v>337</v>
       </c>
-      <c r="E42" s="75">
+      <c r="E42" s="74">
         <v>6</v>
       </c>
       <c r="F42" s="28" t="s">
@@ -7920,16 +7960,16 @@
         <v>354</v>
       </c>
       <c r="C43" s="30"/>
-      <c r="D43" s="76" t="s">
+      <c r="D43" s="75" t="s">
         <v>355</v>
       </c>
-      <c r="E43" s="77">
+      <c r="E43" s="76">
         <v>1</v>
       </c>
       <c r="F43" s="30" t="s">
         <v>201</v>
       </c>
-      <c r="G43" s="76" t="s">
+      <c r="G43" s="75" t="s">
         <v>356</v>
       </c>
       <c r="H43" s="27" t="s">
@@ -7973,16 +8013,16 @@
         <v>223</v>
       </c>
       <c r="C44" s="30"/>
-      <c r="D44" s="76" t="s">
+      <c r="D44" s="75" t="s">
         <v>359</v>
       </c>
-      <c r="E44" s="77">
+      <c r="E44" s="76">
         <v>1</v>
       </c>
       <c r="F44" s="30" t="s">
         <v>201</v>
       </c>
-      <c r="G44" s="76" t="s">
+      <c r="G44" s="75" t="s">
         <v>360</v>
       </c>
       <c r="H44" s="27" t="s">
@@ -8026,16 +8066,16 @@
         <v>364</v>
       </c>
       <c r="C45" s="30"/>
-      <c r="D45" s="76" t="s">
+      <c r="D45" s="75" t="s">
         <v>365</v>
       </c>
-      <c r="E45" s="77">
+      <c r="E45" s="76">
         <v>1</v>
       </c>
       <c r="F45" s="30" t="s">
         <v>201</v>
       </c>
-      <c r="G45" s="76" t="s">
+      <c r="G45" s="75" t="s">
         <v>137</v>
       </c>
       <c r="H45" s="27"/>
@@ -8074,16 +8114,16 @@
         <v>224</v>
       </c>
       <c r="C46" s="30"/>
-      <c r="D46" s="76" t="s">
+      <c r="D46" s="75" t="s">
         <v>367</v>
       </c>
-      <c r="E46" s="77">
+      <c r="E46" s="76">
         <v>1</v>
       </c>
       <c r="F46" s="30" t="s">
         <v>201</v>
       </c>
-      <c r="G46" s="76" t="s">
+      <c r="G46" s="75" t="s">
         <v>368</v>
       </c>
       <c r="H46" s="27" t="s">
@@ -8130,7 +8170,7 @@
       <c r="D47" s="27" t="s">
         <v>373</v>
       </c>
-      <c r="E47" s="75">
+      <c r="E47" s="74">
         <v>1</v>
       </c>
       <c r="F47" s="28" t="s">
@@ -8183,7 +8223,7 @@
       <c r="D48" s="27" t="s">
         <v>379</v>
       </c>
-      <c r="E48" s="75">
+      <c r="E48" s="74">
         <v>2</v>
       </c>
       <c r="F48" s="28" t="s">
@@ -8236,7 +8276,7 @@
       <c r="D49" s="27" t="s">
         <v>384</v>
       </c>
-      <c r="E49" s="75">
+      <c r="E49" s="74">
         <v>1</v>
       </c>
       <c r="F49" s="28" t="s">
@@ -8289,7 +8329,7 @@
       <c r="D50" s="27" t="s">
         <v>388</v>
       </c>
-      <c r="E50" s="75">
+      <c r="E50" s="74">
         <v>1</v>
       </c>
       <c r="F50" s="28" t="s">
@@ -8339,16 +8379,16 @@
         <v>232</v>
       </c>
       <c r="C51" s="30"/>
-      <c r="D51" s="76" t="s">
+      <c r="D51" s="75" t="s">
         <v>393</v>
       </c>
-      <c r="E51" s="77">
+      <c r="E51" s="76">
         <v>1</v>
       </c>
       <c r="F51" s="30" t="s">
         <v>201</v>
       </c>
-      <c r="G51" s="76" t="s">
+      <c r="G51" s="75" t="s">
         <v>394</v>
       </c>
       <c r="H51" s="28" t="s">
@@ -8395,7 +8435,7 @@
       <c r="D52" s="27" t="s">
         <v>398</v>
       </c>
-      <c r="E52" s="75">
+      <c r="E52" s="74">
         <v>1</v>
       </c>
       <c r="F52" s="28" t="s">
@@ -8445,16 +8485,16 @@
         <v>402</v>
       </c>
       <c r="C53" s="30"/>
-      <c r="D53" s="76" t="s">
+      <c r="D53" s="75" t="s">
         <v>403</v>
       </c>
-      <c r="E53" s="77">
+      <c r="E53" s="76">
         <v>1</v>
       </c>
       <c r="F53" s="30" t="s">
         <v>201</v>
       </c>
-      <c r="G53" s="76" t="s">
+      <c r="G53" s="75" t="s">
         <v>404</v>
       </c>
       <c r="H53" s="27"/>
@@ -8496,7 +8536,7 @@
       <c r="D54" s="27" t="s">
         <v>262</v>
       </c>
-      <c r="E54" s="75">
+      <c r="E54" s="74">
         <v>2</v>
       </c>
       <c r="F54" s="28" t="s">
@@ -8536,12 +8576,12 @@
       <c r="A55" s="27">
         <v>105</v>
       </c>
-      <c r="B55" s="76" t="s">
+      <c r="B55" s="75" t="s">
         <v>142</v>
       </c>
-      <c r="C55" s="76"/>
+      <c r="C55" s="75"/>
       <c r="D55" s="30"/>
-      <c r="E55" s="77">
+      <c r="E55" s="76">
         <v>1</v>
       </c>
       <c r="F55" s="30" t="s">
@@ -8577,14 +8617,14 @@
       <c r="A56" s="27">
         <v>106</v>
       </c>
-      <c r="B56" s="83" t="s">
+      <c r="B56" s="82" t="s">
         <v>415</v>
       </c>
-      <c r="C56" s="83"/>
-      <c r="D56" s="84" t="s">
+      <c r="C56" s="82"/>
+      <c r="D56" s="83" t="s">
         <v>439</v>
       </c>
-      <c r="E56" s="75">
+      <c r="E56" s="74">
         <v>1</v>
       </c>
       <c r="F56" s="28" t="s">
@@ -8592,7 +8632,7 @@
       </c>
     </row>
     <row r="57" spans="1:20" s="39" customFormat="1" ht="24" x14ac:dyDescent="0.15">
-      <c r="A57" s="69" t="s">
+      <c r="A57" s="68" t="s">
         <v>487</v>
       </c>
       <c r="R57" s="40"/>
@@ -8601,10 +8641,10 @@
       <c r="A58" s="27">
         <v>107</v>
       </c>
-      <c r="B58" s="85" t="s">
+      <c r="B58" s="84" t="s">
         <v>435</v>
       </c>
-      <c r="C58" s="85"/>
+      <c r="C58" s="84"/>
       <c r="K58" s="27">
         <f>IF(J58&gt;E58,0,E58-J58)</f>
         <v>0</v>
@@ -8626,10 +8666,10 @@
       <c r="A59" s="27">
         <v>108</v>
       </c>
-      <c r="B59" s="85" t="s">
+      <c r="B59" s="84" t="s">
         <v>436</v>
       </c>
-      <c r="C59" s="85"/>
+      <c r="C59" s="84"/>
       <c r="K59" s="27">
         <f>IF(J59&gt;E59,0,E59-J59)</f>
         <v>0</v>
@@ -8651,10 +8691,10 @@
       <c r="A60" s="27">
         <v>109</v>
       </c>
-      <c r="B60" s="85" t="s">
+      <c r="B60" s="84" t="s">
         <v>437</v>
       </c>
-      <c r="C60" s="85"/>
+      <c r="C60" s="84"/>
       <c r="K60" s="27">
         <f>IF(J60&gt;E60,0,E60-J60)</f>
         <v>0</v>
@@ -8673,400 +8713,424 @@
       </c>
     </row>
     <row r="61" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="B61" s="82" t="s">
-        <v>506</v>
-      </c>
-      <c r="C61" s="85"/>
+      <c r="B61" s="92" t="s">
+        <v>536</v>
+      </c>
+      <c r="C61" s="84"/>
     </row>
     <row r="62" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="B62" s="82" t="s">
-        <v>507</v>
-      </c>
-      <c r="C62" s="85"/>
-    </row>
-    <row r="63" spans="1:20" s="39" customFormat="1" ht="24" x14ac:dyDescent="0.15">
-      <c r="A63" s="69" t="s">
+      <c r="B62" s="92" t="s">
+        <v>537</v>
+      </c>
+      <c r="C62" s="84"/>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="B63" s="92" t="s">
+        <v>531</v>
+      </c>
+      <c r="C63" s="84"/>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="B64" s="92" t="s">
+        <v>530</v>
+      </c>
+      <c r="C64" s="84"/>
+    </row>
+    <row r="65" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="B65" s="92" t="s">
+        <v>529</v>
+      </c>
+      <c r="C65" s="84"/>
+    </row>
+    <row r="66" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="B66" s="92" t="s">
+        <v>532</v>
+      </c>
+      <c r="C66" s="84"/>
+    </row>
+    <row r="67" spans="1:20" s="39" customFormat="1" ht="24" x14ac:dyDescent="0.15">
+      <c r="A67" s="68" t="s">
         <v>484</v>
       </c>
-      <c r="R63" s="40"/>
-    </row>
-    <row r="64" spans="1:20" s="86" customFormat="1" ht="17" x14ac:dyDescent="0.15">
-      <c r="B64" s="55"/>
-      <c r="C64" s="87" t="s">
+      <c r="R67" s="40"/>
+    </row>
+    <row r="68" spans="1:20" s="85" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+      <c r="B68" s="55"/>
+      <c r="C68" s="86" t="s">
         <v>508</v>
       </c>
-      <c r="E64" s="88">
-        <v>1</v>
-      </c>
-      <c r="F64" s="67" t="s">
+      <c r="E68" s="87">
+        <v>1</v>
+      </c>
+      <c r="F68" s="66" t="s">
         <v>201</v>
       </c>
-      <c r="G64" s="87" t="s">
+      <c r="G68" s="86" t="s">
         <v>528</v>
       </c>
-      <c r="H64" s="87" t="s">
+      <c r="H68" s="86" t="s">
         <v>527</v>
       </c>
-      <c r="K64" s="55"/>
-      <c r="L64" s="55"/>
-      <c r="M64" s="55"/>
-      <c r="N64" s="55"/>
-      <c r="O64" s="55"/>
-      <c r="P64" s="55">
+      <c r="K68" s="55"/>
+      <c r="L68" s="55"/>
+      <c r="M68" s="55"/>
+      <c r="N68" s="55"/>
+      <c r="O68" s="55"/>
+      <c r="P68" s="55">
         <v>21.88</v>
       </c>
-      <c r="Q64" s="55">
+      <c r="Q68" s="55">
         <v>21.88</v>
       </c>
-      <c r="R64" s="55">
+      <c r="R68" s="55">
         <v>21.88</v>
       </c>
-      <c r="S64" s="86" t="s">
+      <c r="S68" s="85" t="s">
         <v>317</v>
       </c>
-      <c r="T64" s="86" t="s">
+      <c r="T68" s="85" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="65" spans="1:20" s="86" customFormat="1" ht="17" x14ac:dyDescent="0.15">
-      <c r="B65" s="55"/>
-      <c r="C65" s="87" t="s">
+    <row r="69" spans="1:20" s="85" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+      <c r="B69" s="55"/>
+      <c r="C69" s="86" t="s">
         <v>526</v>
       </c>
-      <c r="D65" s="87" t="s">
+      <c r="D69" s="86" t="s">
         <v>519</v>
       </c>
-      <c r="E65" s="88">
+      <c r="E69" s="87">
         <v>2</v>
       </c>
-      <c r="F65" s="67" t="s">
+      <c r="F69" s="66" t="s">
         <v>201</v>
       </c>
-      <c r="G65" s="87" t="s">
+      <c r="G69" s="86" t="s">
         <v>525</v>
       </c>
-      <c r="H65" s="87" t="s">
+      <c r="H69" s="86" t="s">
         <v>524</v>
       </c>
-      <c r="K65" s="55"/>
-      <c r="L65" s="55"/>
-      <c r="M65" s="55"/>
-      <c r="N65" s="55"/>
-      <c r="O65" s="55"/>
-      <c r="P65" s="55"/>
-      <c r="Q65" s="55"/>
-      <c r="R65" s="55"/>
-    </row>
-    <row r="66" spans="1:20" s="86" customFormat="1" ht="17" x14ac:dyDescent="0.15">
-      <c r="B66" s="55"/>
-      <c r="C66" s="87" t="s">
+      <c r="K69" s="55"/>
+      <c r="L69" s="55"/>
+      <c r="M69" s="55"/>
+      <c r="N69" s="55"/>
+      <c r="O69" s="55"/>
+      <c r="P69" s="55"/>
+      <c r="Q69" s="55"/>
+      <c r="R69" s="55"/>
+    </row>
+    <row r="70" spans="1:20" s="85" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+      <c r="B70" s="55"/>
+      <c r="C70" s="86" t="s">
         <v>521</v>
       </c>
-      <c r="D66" s="87" t="s">
+      <c r="D70" s="86" t="s">
         <v>523</v>
       </c>
-      <c r="E66" s="88">
-        <v>1</v>
-      </c>
-      <c r="F66" s="67" t="s">
+      <c r="E70" s="87">
+        <v>1</v>
+      </c>
+      <c r="F70" s="66" t="s">
         <v>201</v>
       </c>
-      <c r="G66" s="87" t="s">
+      <c r="G70" s="86" t="s">
         <v>522</v>
       </c>
-      <c r="H66" s="87" t="s">
+      <c r="H70" s="86" t="s">
         <v>520</v>
       </c>
-      <c r="K66" s="55"/>
-      <c r="L66" s="55"/>
-      <c r="M66" s="55"/>
-      <c r="N66" s="55"/>
-      <c r="O66" s="55"/>
-      <c r="P66" s="55"/>
-      <c r="Q66" s="55"/>
-      <c r="R66" s="55"/>
-    </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="B67" s="28"/>
-      <c r="D67" s="27"/>
-      <c r="E67" s="75"/>
-      <c r="G67" s="27"/>
-      <c r="H67" s="27"/>
-      <c r="K67" s="28"/>
-      <c r="L67" s="28"/>
-      <c r="M67" s="28"/>
-      <c r="N67" s="28"/>
-      <c r="O67" s="28"/>
-    </row>
-    <row r="68" spans="1:20" s="39" customFormat="1" ht="24" x14ac:dyDescent="0.15">
-      <c r="A68" s="69" t="s">
+      <c r="K70" s="55"/>
+      <c r="L70" s="55"/>
+      <c r="M70" s="55"/>
+      <c r="N70" s="55"/>
+      <c r="O70" s="55"/>
+      <c r="P70" s="55"/>
+      <c r="Q70" s="55"/>
+      <c r="R70" s="55"/>
+    </row>
+    <row r="71" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="B71" s="28"/>
+      <c r="D71" s="27"/>
+      <c r="E71" s="74"/>
+      <c r="G71" s="27"/>
+      <c r="H71" s="27"/>
+      <c r="K71" s="28"/>
+      <c r="L71" s="28"/>
+      <c r="M71" s="28"/>
+      <c r="N71" s="28"/>
+      <c r="O71" s="28"/>
+    </row>
+    <row r="72" spans="1:20" s="39" customFormat="1" ht="24" x14ac:dyDescent="0.15">
+      <c r="A72" s="68" t="s">
         <v>485</v>
       </c>
-      <c r="D68" s="70"/>
-      <c r="G68" s="71"/>
-      <c r="H68" s="71"/>
-      <c r="I68" s="70"/>
-      <c r="R68" s="40"/>
-    </row>
-    <row r="69" spans="1:20" ht="17" x14ac:dyDescent="0.15">
-      <c r="A69" s="27">
+      <c r="D72" s="69"/>
+      <c r="G72" s="70"/>
+      <c r="H72" s="70"/>
+      <c r="I72" s="69"/>
+      <c r="R72" s="40"/>
+    </row>
+    <row r="73" spans="1:20" ht="17" x14ac:dyDescent="0.15">
+      <c r="A73" s="27">
         <v>103</v>
       </c>
-      <c r="B69" s="28" t="s">
+      <c r="B73" s="28" t="s">
         <v>410</v>
       </c>
-      <c r="D69" s="27" t="s">
+      <c r="D73" s="27" t="s">
         <v>314</v>
       </c>
-      <c r="E69" s="75">
+      <c r="E73" s="74">
         <v>2</v>
       </c>
-      <c r="F69" s="28" t="s">
+      <c r="F73" s="28" t="s">
         <v>201</v>
       </c>
-      <c r="G69" s="27" t="s">
+      <c r="G73" s="27" t="s">
         <v>315</v>
       </c>
-      <c r="H69" s="27" t="s">
+      <c r="H73" s="27" t="s">
         <v>316</v>
       </c>
-      <c r="I69" s="27" t="s">
+      <c r="I73" s="27" t="s">
         <v>204</v>
       </c>
-      <c r="J69" s="27">
+      <c r="J73" s="27">
         <v>2</v>
       </c>
-      <c r="K69" s="28">
-        <f>IF(J69&gt;E69,0,E69-J69)</f>
-        <v>0</v>
-      </c>
-      <c r="L69" s="28">
-        <f>J69+K69</f>
+      <c r="K73" s="28">
+        <f>IF(J73&gt;E73,0,E73-J73)</f>
+        <v>0</v>
+      </c>
+      <c r="L73" s="28">
+        <f>J73+K73</f>
         <v>2</v>
       </c>
-      <c r="M69" s="28">
-        <f>L69-E69</f>
-        <v>0</v>
-      </c>
-      <c r="N69" s="28">
-        <f>(4*E69)-M69</f>
+      <c r="M73" s="28">
+        <f>L73-E73</f>
+        <v>0</v>
+      </c>
+      <c r="N73" s="28">
+        <f>(4*E73)-M73</f>
         <v>8</v>
       </c>
-      <c r="O69" s="28"/>
-      <c r="S69" s="27" t="s">
+      <c r="O73" s="28"/>
+      <c r="S73" s="27" t="s">
         <v>317</v>
       </c>
-      <c r="T69" s="27" t="s">
+      <c r="T73" s="27" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="70" spans="1:20" ht="17" x14ac:dyDescent="0.15">
-      <c r="A70" s="27">
+    <row r="74" spans="1:20" ht="17" x14ac:dyDescent="0.15">
+      <c r="A74" s="27">
         <v>104</v>
       </c>
-      <c r="B70" s="27" t="s">
+      <c r="B74" s="27" t="s">
         <v>410</v>
       </c>
-      <c r="D70" s="28" t="s">
+      <c r="D74" s="28" t="s">
         <v>411</v>
       </c>
-      <c r="E70" s="75">
-        <v>1</v>
-      </c>
-      <c r="F70" s="28" t="s">
+      <c r="E74" s="74">
+        <v>1</v>
+      </c>
+      <c r="F74" s="28" t="s">
         <v>201</v>
       </c>
-      <c r="G70" s="28" t="s">
+      <c r="G74" s="28" t="s">
         <v>412</v>
       </c>
-      <c r="H70" s="28" t="s">
+      <c r="H74" s="28" t="s">
         <v>413</v>
       </c>
-      <c r="I70" s="27" t="s">
+      <c r="I74" s="27" t="s">
         <v>204</v>
       </c>
-      <c r="J70" s="27">
-        <v>1</v>
-      </c>
-      <c r="K70" s="27">
-        <f>IF(J70&gt;E70,0,E70-J70)</f>
-        <v>0</v>
-      </c>
-      <c r="L70" s="27">
-        <f>J70+K70</f>
-        <v>1</v>
-      </c>
-      <c r="M70" s="27">
-        <f>L70-E70</f>
-        <v>0</v>
-      </c>
-      <c r="N70" s="27">
-        <f>(4*E70)-M70</f>
+      <c r="J74" s="27">
+        <v>1</v>
+      </c>
+      <c r="K74" s="27">
+        <f>IF(J74&gt;E74,0,E74-J74)</f>
+        <v>0</v>
+      </c>
+      <c r="L74" s="27">
+        <f>J74+K74</f>
+        <v>1</v>
+      </c>
+      <c r="M74" s="27">
+        <f>L74-E74</f>
+        <v>0</v>
+      </c>
+      <c r="N74" s="27">
+        <f>(4*E74)-M74</f>
         <v>4</v>
       </c>
     </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="E71" s="75"/>
-    </row>
-    <row r="72" spans="1:20" ht="17" x14ac:dyDescent="0.15">
-      <c r="C72" s="89" t="s">
+    <row r="75" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="E75" s="74"/>
+    </row>
+    <row r="76" spans="1:20" ht="17" x14ac:dyDescent="0.15">
+      <c r="C76" s="88" t="s">
         <v>505</v>
       </c>
-      <c r="D72" s="74" t="s">
+      <c r="D76" s="73" t="s">
         <v>502</v>
       </c>
-      <c r="E72" s="81">
+      <c r="E76" s="80">
         <v>2</v>
       </c>
-      <c r="F72" s="74" t="s">
+      <c r="F76" s="73" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="73" spans="1:20" ht="17" x14ac:dyDescent="0.15">
-      <c r="C73" s="89" t="s">
+    <row r="77" spans="1:20" ht="17" x14ac:dyDescent="0.15">
+      <c r="C77" s="88" t="s">
         <v>505</v>
       </c>
-      <c r="D73" s="74" t="s">
+      <c r="D77" s="73" t="s">
         <v>503</v>
       </c>
-      <c r="E73" s="81">
-        <v>1</v>
-      </c>
-      <c r="F73" s="74" t="s">
+      <c r="E77" s="80">
+        <v>1</v>
+      </c>
+      <c r="F77" s="73" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="74" spans="1:20" ht="17" x14ac:dyDescent="0.15">
-      <c r="C74" s="89" t="s">
+    <row r="78" spans="1:20" ht="17" x14ac:dyDescent="0.15">
+      <c r="C78" s="88" t="s">
         <v>505</v>
       </c>
-      <c r="D74" s="74" t="s">
+      <c r="D78" s="73" t="s">
         <v>500</v>
       </c>
-      <c r="E74" s="81">
-        <v>1</v>
-      </c>
-      <c r="F74" s="74" t="s">
+      <c r="E78" s="80">
+        <v>1</v>
+      </c>
+      <c r="F78" s="73" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="75" spans="1:20" ht="17" x14ac:dyDescent="0.15">
-      <c r="C75" s="89" t="s">
+    <row r="79" spans="1:20" ht="17" x14ac:dyDescent="0.15">
+      <c r="C79" s="88" t="s">
         <v>505</v>
       </c>
-      <c r="D75" s="74" t="s">
+      <c r="D79" s="73" t="s">
         <v>501</v>
       </c>
-      <c r="E75" s="81">
-        <v>1</v>
-      </c>
-      <c r="F75" s="74" t="s">
+      <c r="E79" s="80">
+        <v>1</v>
+      </c>
+      <c r="F79" s="73" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="C76" s="90" t="s">
+    <row r="80" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="C80" s="89" t="s">
         <v>516</v>
       </c>
-      <c r="D76" s="74"/>
-      <c r="E76" s="81"/>
-      <c r="F76" s="74"/>
-    </row>
-    <row r="77" spans="1:20" s="86" customFormat="1" ht="17" x14ac:dyDescent="0.15">
-      <c r="C77" s="89" t="s">
+      <c r="D80" s="73"/>
+      <c r="E80" s="80"/>
+      <c r="F80" s="73"/>
+    </row>
+    <row r="81" spans="1:18" s="85" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+      <c r="C81" s="88" t="s">
         <v>514</v>
       </c>
-      <c r="D77" s="74" t="s">
+      <c r="D81" s="73" t="s">
         <v>515</v>
       </c>
-      <c r="E77" s="81">
+      <c r="E81" s="80">
         <v>2</v>
       </c>
-      <c r="F77" s="74" t="s">
+      <c r="F81" s="73" t="s">
         <v>201</v>
       </c>
-      <c r="G77" s="67" t="s">
+      <c r="G81" s="66" t="s">
         <v>518</v>
       </c>
-      <c r="H77" s="67" t="s">
+      <c r="H81" s="66" t="s">
         <v>517</v>
       </c>
-      <c r="P77" s="55"/>
-      <c r="Q77" s="55"/>
-      <c r="R77" s="55"/>
-    </row>
-    <row r="78" spans="1:20" s="86" customFormat="1" ht="85" x14ac:dyDescent="0.15">
-      <c r="C78" s="67" t="s">
+      <c r="P81" s="55"/>
+      <c r="Q81" s="55"/>
+      <c r="R81" s="55"/>
+    </row>
+    <row r="82" spans="1:18" s="85" customFormat="1" ht="85" x14ac:dyDescent="0.15">
+      <c r="C82" s="66" t="s">
         <v>504</v>
       </c>
-      <c r="D78" s="67" t="s">
+      <c r="D82" s="66" t="s">
         <v>498</v>
       </c>
-      <c r="E78" s="88"/>
-      <c r="F78" s="55"/>
-      <c r="G78" s="55" t="s">
+      <c r="E82" s="87"/>
+      <c r="F82" s="55"/>
+      <c r="G82" s="55" t="s">
         <v>497</v>
       </c>
-      <c r="H78" s="67" t="s">
+      <c r="H82" s="66" t="s">
         <v>499</v>
       </c>
-      <c r="P78" s="55"/>
-      <c r="Q78" s="55"/>
-      <c r="R78" s="55"/>
-    </row>
-    <row r="79" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A79" s="27">
+      <c r="P82" s="55"/>
+      <c r="Q82" s="55"/>
+      <c r="R82" s="55"/>
+    </row>
+    <row r="83" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A83" s="27">
         <v>101</v>
       </c>
-      <c r="B79" s="91" t="s">
+      <c r="B83" s="90" t="s">
         <v>430</v>
       </c>
-      <c r="C79" s="91"/>
-      <c r="E79" s="75">
-        <v>1</v>
-      </c>
-      <c r="G79" s="27" t="s">
+      <c r="C83" s="90"/>
+      <c r="E83" s="74">
+        <v>1</v>
+      </c>
+      <c r="G83" s="27" t="s">
         <v>406</v>
       </c>
-      <c r="H79" s="27" t="s">
+      <c r="H83" s="27" t="s">
         <v>407</v>
       </c>
-      <c r="I79" s="27" t="s">
+      <c r="I83" s="27" t="s">
         <v>220</v>
       </c>
-      <c r="J79" s="27">
-        <v>0</v>
-      </c>
-      <c r="K79" s="30">
-        <f>IF(J79&gt;E79,0,E79-J79)</f>
-        <v>1</v>
-      </c>
-      <c r="L79" s="28">
-        <f>J79+K79</f>
-        <v>1</v>
-      </c>
-      <c r="M79" s="28">
-        <f>L79-E79</f>
-        <v>0</v>
-      </c>
-      <c r="N79" s="28">
-        <f>(4*E79)-M79</f>
+      <c r="J83" s="27">
+        <v>0</v>
+      </c>
+      <c r="K83" s="30">
+        <f>IF(J83&gt;E83,0,E83-J83)</f>
+        <v>1</v>
+      </c>
+      <c r="L83" s="28">
+        <f>J83+K83</f>
+        <v>1</v>
+      </c>
+      <c r="M83" s="28">
+        <f>L83-E83</f>
+        <v>0</v>
+      </c>
+      <c r="N83" s="28">
+        <f>(4*E83)-M83</f>
         <v>4</v>
       </c>
-      <c r="O79" s="28"/>
-    </row>
-    <row r="80" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="C80" s="82" t="s">
+      <c r="O83" s="28"/>
+    </row>
+    <row r="84" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="C84" s="81" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="81" spans="3:3" x14ac:dyDescent="0.15">
-      <c r="C81" s="82" t="s">
+    <row r="85" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="C85" s="81" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="82" spans="3:3" x14ac:dyDescent="0.15">
-      <c r="C82" s="82" t="s">
+    <row r="86" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="C86" s="81" t="s">
         <v>513</v>
       </c>
     </row>
@@ -9074,7 +9138,7 @@
   <mergeCells count="1">
     <mergeCell ref="P7:R7"/>
   </mergeCells>
-  <phoneticPr fontId="16" type="noConversion"/>
+  <phoneticPr fontId="17" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -9084,7 +9148,7 @@
   <dimension ref="A1:R30"/>
   <sheetViews>
     <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.15"/>
@@ -9126,11 +9190,11 @@
         <v>173</v>
       </c>
       <c r="C3" s="27"/>
-      <c r="P3" s="66" t="s">
+      <c r="P3" s="91" t="s">
         <v>174</v>
       </c>
-      <c r="Q3" s="66"/>
-      <c r="R3" s="66"/>
+      <c r="Q3" s="91"/>
+      <c r="R3" s="91"/>
     </row>
     <row r="4" spans="1:18" ht="17" x14ac:dyDescent="0.15">
       <c r="A4" s="29"/>
@@ -9192,7 +9256,7 @@
       <c r="B6" s="28" t="s">
         <v>189</v>
       </c>
-      <c r="C6" s="72" t="s">
+      <c r="C6" s="71" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="28" t="s">
@@ -9559,13 +9623,22 @@
       </c>
       <c r="R18" s="40"/>
     </row>
-    <row r="19" spans="1:18" s="39" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:18" s="39" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+      <c r="D19" s="93" t="s">
+        <v>533</v>
+      </c>
       <c r="R19" s="40"/>
     </row>
-    <row r="20" spans="1:18" s="39" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:18" s="39" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+      <c r="D20" s="93" t="s">
+        <v>534</v>
+      </c>
       <c r="R20" s="40"/>
     </row>
-    <row r="21" spans="1:18" s="39" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:18" s="39" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+      <c r="D21" s="93" t="s">
+        <v>535</v>
+      </c>
       <c r="R21" s="40"/>
     </row>
     <row r="22" spans="1:18" s="39" customFormat="1" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Add regulator and battery connector data sheets, footprints, symbols
</commit_message>
<xml_diff>
--- a/Manufacturing/BOM Core 64 v0.4.0 Yellow Dual Boards.xlsx
+++ b/Manufacturing/BOM Core 64 v0.4.0 Yellow Dual Boards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ageppert/Dropbox/Electronics/Core 64 Interactive Badge/Core-64-Interactive-Core-Memory-Badge/Manufacturing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AE441FD-BA06-FE46-B329-29821F6E67BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7AD73FC-AE0D-0340-A605-571D9E2E2C03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="27480" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1700,10 +1700,17 @@
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.000_);_(&quot;$&quot;* \(#,##0.000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1936,36 +1943,36 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="15" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="14" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="13" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1975,154 +1982,81 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="11" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="11" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="11" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="16" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="15" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="17" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="16" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="11" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -2130,68 +2064,153 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="12" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -4947,8 +4966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F5DBFB5-E21A-7B4B-815F-748A526FD280}">
   <dimension ref="A1:R37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="125" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.15"/>
@@ -4991,11 +5010,11 @@
         <v>172</v>
       </c>
       <c r="C3" s="27"/>
-      <c r="P3" s="86" t="s">
+      <c r="P3" s="99" t="s">
         <v>173</v>
       </c>
-      <c r="Q3" s="86"/>
-      <c r="R3" s="86"/>
+      <c r="Q3" s="99"/>
+      <c r="R3" s="99"/>
     </row>
     <row r="4" spans="1:18" ht="51" x14ac:dyDescent="0.15">
       <c r="A4" s="29"/>
@@ -5016,7 +5035,7 @@
         <v>176</v>
       </c>
       <c r="C5" s="38"/>
-      <c r="D5" s="38" t="s">
+      <c r="D5" s="30" t="s">
         <v>177</v>
       </c>
       <c r="E5" s="38"/>
@@ -5028,7 +5047,7 @@
       <c r="K5" s="38" t="s">
         <v>180</v>
       </c>
-      <c r="L5" s="87" t="s">
+      <c r="L5" s="86" t="s">
         <v>527</v>
       </c>
       <c r="M5" s="53" t="s">
@@ -5742,53 +5761,56 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="26" spans="1:18" ht="34" x14ac:dyDescent="0.15">
-      <c r="A26" s="53" t="s">
+    <row r="26" spans="1:18" s="30" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+      <c r="A26" s="100" t="s">
         <v>443</v>
       </c>
-      <c r="B26" s="54" t="s">
+      <c r="B26" s="30" t="s">
         <v>217</v>
       </c>
-      <c r="C26" s="64" t="s">
+      <c r="C26" s="90" t="s">
         <v>487</v>
       </c>
-      <c r="D26" s="55" t="s">
+      <c r="D26" s="100" t="s">
         <v>444</v>
       </c>
-      <c r="E26" s="54">
+      <c r="E26" s="30">
         <v>4</v>
       </c>
-      <c r="F26" s="54" t="s">
+      <c r="F26" s="30" t="s">
         <v>200</v>
       </c>
-      <c r="G26" s="59" t="s">
+      <c r="G26" s="101" t="s">
         <v>459</v>
       </c>
-      <c r="H26" s="55" t="s">
+      <c r="H26" s="100" t="s">
         <v>458</v>
       </c>
-      <c r="I26" s="59" t="s">
+      <c r="I26" s="101" t="s">
         <v>203</v>
       </c>
-      <c r="J26" s="28">
-        <v>0</v>
-      </c>
-      <c r="K26" s="54">
+      <c r="J26" s="30">
+        <v>0</v>
+      </c>
+      <c r="K26" s="30">
         <f t="shared" ref="K26" si="7">IF(J26&gt;E26,0,E26-J26)</f>
         <v>4</v>
       </c>
-      <c r="M26" s="28">
+      <c r="L26" s="30">
+        <v>4</v>
+      </c>
+      <c r="M26" s="30">
         <f t="shared" ref="M26" si="8">L26-E26</f>
-        <v>-4</v>
-      </c>
-      <c r="N26" s="28">
+        <v>0</v>
+      </c>
+      <c r="N26" s="30">
         <f t="shared" ref="N26" si="9">(4*E26)-M26</f>
-        <v>20</v>
-      </c>
-      <c r="R26" s="32"/>
-    </row>
-    <row r="27" spans="1:18" ht="34" x14ac:dyDescent="0.15">
-      <c r="A27" s="60" t="s">
+        <v>16</v>
+      </c>
+      <c r="R26" s="102"/>
+    </row>
+    <row r="27" spans="1:18" s="54" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+      <c r="A27" s="59" t="s">
         <v>472</v>
       </c>
       <c r="B27" s="54" t="s">
@@ -5815,25 +5837,25 @@
       <c r="I27" s="55" t="s">
         <v>219</v>
       </c>
-      <c r="J27" s="28">
+      <c r="J27" s="54">
         <v>0</v>
       </c>
       <c r="K27" s="54">
         <f>IF(J27&gt;E27,0,E27-J27)</f>
         <v>4</v>
       </c>
-      <c r="L27" s="28">
+      <c r="L27" s="54">
         <v>4</v>
       </c>
-      <c r="M27" s="28">
+      <c r="M27" s="54">
         <f t="shared" ref="M27:M32" si="10">L27-E27</f>
         <v>0</v>
       </c>
-      <c r="N27" s="28">
+      <c r="N27" s="54">
         <f t="shared" ref="N27:N32" si="11">(4*E27)-M27</f>
         <v>16</v>
       </c>
-      <c r="R27" s="32"/>
+      <c r="R27" s="103"/>
     </row>
     <row r="28" spans="1:18" ht="17" x14ac:dyDescent="0.15">
       <c r="A28" s="28">
@@ -6330,14 +6352,14 @@
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.15">
-      <c r="P7" s="86" t="s">
+      <c r="P7" s="99" t="s">
         <v>173</v>
       </c>
-      <c r="Q7" s="86"/>
-      <c r="R7" s="86"/>
-    </row>
-    <row r="8" spans="1:31" s="95" customFormat="1" ht="17" x14ac:dyDescent="0.15">
-      <c r="A8" s="95" t="s">
+      <c r="Q7" s="99"/>
+      <c r="R7" s="99"/>
+    </row>
+    <row r="8" spans="1:31" s="94" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+      <c r="A8" s="94" t="s">
         <v>243</v>
       </c>
       <c r="D8" s="38"/>
@@ -6354,11 +6376,11 @@
       <c r="M8" s="38"/>
       <c r="N8" s="38"/>
       <c r="O8" s="38"/>
-      <c r="P8" s="99"/>
-      <c r="Q8" s="99"/>
-      <c r="R8" s="99"/>
-    </row>
-    <row r="9" spans="1:31" s="95" customFormat="1" ht="51" x14ac:dyDescent="0.15">
+      <c r="P8" s="98"/>
+      <c r="Q8" s="98"/>
+      <c r="R8" s="98"/>
+    </row>
+    <row r="9" spans="1:31" s="94" customFormat="1" ht="51" x14ac:dyDescent="0.15">
       <c r="B9" s="38" t="s">
         <v>176</v>
       </c>
@@ -6400,8 +6422,8 @@
         <v>186</v>
       </c>
     </row>
-    <row r="10" spans="1:31" s="95" customFormat="1" ht="17" x14ac:dyDescent="0.15">
-      <c r="A10" s="95" t="s">
+    <row r="10" spans="1:31" s="94" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+      <c r="A10" s="94" t="s">
         <v>413</v>
       </c>
       <c r="B10" s="38" t="s">
@@ -6410,22 +6432,22 @@
       <c r="C10" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="95" t="s">
+      <c r="D10" s="94" t="s">
         <v>245</v>
       </c>
-      <c r="E10" s="97" t="s">
+      <c r="E10" s="96" t="s">
         <v>246</v>
       </c>
       <c r="F10" s="38" t="s">
         <v>190</v>
       </c>
-      <c r="G10" s="95" t="s">
+      <c r="G10" s="94" t="s">
         <v>247</v>
       </c>
       <c r="H10" s="38" t="s">
         <v>191</v>
       </c>
-      <c r="I10" s="95" t="s">
+      <c r="I10" s="94" t="s">
         <v>248</v>
       </c>
       <c r="J10" s="38" t="s">
@@ -6453,70 +6475,70 @@
       <c r="R10" s="38" t="s">
         <v>199</v>
       </c>
-      <c r="S10" s="95" t="s">
+      <c r="S10" s="94" t="s">
         <v>249</v>
       </c>
-      <c r="T10" s="95" t="s">
+      <c r="T10" s="94" t="s">
         <v>250</v>
       </c>
-      <c r="U10" s="95" t="s">
+      <c r="U10" s="94" t="s">
         <v>251</v>
       </c>
-      <c r="V10" s="95" t="s">
+      <c r="V10" s="94" t="s">
         <v>252</v>
       </c>
-      <c r="W10" s="95" t="s">
+      <c r="W10" s="94" t="s">
         <v>253</v>
       </c>
-      <c r="X10" s="95" t="s">
+      <c r="X10" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="Y10" s="95" t="s">
+      <c r="Y10" s="94" t="s">
         <v>254</v>
       </c>
-      <c r="Z10" s="95" t="s">
+      <c r="Z10" s="94" t="s">
         <v>255</v>
       </c>
-      <c r="AA10" s="95" t="s">
+      <c r="AA10" s="94" t="s">
         <v>256</v>
       </c>
-      <c r="AB10" s="95" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC10" s="95" t="s">
+      <c r="AB10" s="94" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC10" s="94" t="s">
         <v>257</v>
       </c>
-      <c r="AD10" s="95" t="s">
+      <c r="AD10" s="94" t="s">
         <v>258</v>
       </c>
-      <c r="AE10" s="95" t="s">
+      <c r="AE10" s="94" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="11" spans="1:31" s="95" customFormat="1" ht="17" x14ac:dyDescent="0.15">
-      <c r="A11" s="95">
+    <row r="11" spans="1:31" s="94" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+      <c r="A11" s="94">
         <v>1</v>
       </c>
       <c r="B11" s="38" t="s">
         <v>260</v>
       </c>
       <c r="C11" s="38"/>
-      <c r="D11" s="95" t="s">
+      <c r="D11" s="94" t="s">
         <v>261</v>
       </c>
-      <c r="E11" s="97">
+      <c r="E11" s="96">
         <v>2</v>
       </c>
       <c r="F11" s="38" t="s">
         <v>200</v>
       </c>
-      <c r="G11" s="95" t="s">
+      <c r="G11" s="94" t="s">
         <v>262</v>
       </c>
-      <c r="H11" s="95" t="s">
+      <c r="H11" s="94" t="s">
         <v>263</v>
       </c>
-      <c r="I11" s="95" t="s">
+      <c r="I11" s="94" t="s">
         <v>203</v>
       </c>
       <c r="J11" s="38">
@@ -6527,55 +6549,55 @@
         <v>2</v>
       </c>
       <c r="L11" s="38">
-        <f>J11+K11</f>
+        <f t="shared" ref="L11:L17" si="0">J11+K11</f>
         <v>2</v>
       </c>
       <c r="M11" s="38">
-        <f>L11-E11</f>
+        <f t="shared" ref="M11:M17" si="1">L11-E11</f>
         <v>0</v>
       </c>
       <c r="N11" s="38">
-        <f>(4*E11)-M11</f>
+        <f t="shared" ref="N11:N17" si="2">(4*E11)-M11</f>
         <v>8</v>
       </c>
       <c r="O11" s="38"/>
       <c r="P11" s="38"/>
       <c r="Q11" s="38"/>
       <c r="R11" s="39" t="e">
-        <f>Q11/P11</f>
+        <f t="shared" ref="R11:R28" si="3">Q11/P11</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="S11" s="95" t="s">
+      <c r="S11" s="94" t="s">
         <v>264</v>
       </c>
-      <c r="T11" s="95" t="s">
+      <c r="T11" s="94" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="12" spans="1:31" s="95" customFormat="1" ht="17" x14ac:dyDescent="0.15">
-      <c r="A12" s="95">
+    <row r="12" spans="1:31" s="94" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+      <c r="A12" s="94">
         <v>2</v>
       </c>
       <c r="B12" s="38" t="s">
         <v>266</v>
       </c>
       <c r="C12" s="38"/>
-      <c r="D12" s="95" t="s">
+      <c r="D12" s="94" t="s">
         <v>267</v>
       </c>
-      <c r="E12" s="97">
+      <c r="E12" s="96">
         <v>7</v>
       </c>
       <c r="F12" s="38" t="s">
         <v>200</v>
       </c>
-      <c r="G12" s="95" t="s">
+      <c r="G12" s="94" t="s">
         <v>201</v>
       </c>
-      <c r="H12" s="95" t="s">
+      <c r="H12" s="94" t="s">
         <v>202</v>
       </c>
-      <c r="I12" s="95" t="s">
+      <c r="I12" s="94" t="s">
         <v>203</v>
       </c>
       <c r="J12" s="38">
@@ -6586,55 +6608,55 @@
         <v>7</v>
       </c>
       <c r="L12" s="38">
-        <f>J12+K12</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="M12" s="38">
-        <f>L12-E12</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N12" s="38">
-        <f>(4*E12)-M12</f>
+        <f t="shared" si="2"/>
         <v>28</v>
       </c>
       <c r="O12" s="38"/>
       <c r="P12" s="38"/>
       <c r="Q12" s="38"/>
       <c r="R12" s="39" t="e">
-        <f>Q12/P12</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="S12" s="95" t="s">
+      <c r="S12" s="94" t="s">
         <v>264</v>
       </c>
-      <c r="T12" s="95" t="s">
+      <c r="T12" s="94" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="13" spans="1:31" s="95" customFormat="1" ht="17" x14ac:dyDescent="0.15">
-      <c r="A13" s="95">
+    <row r="13" spans="1:31" s="94" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+      <c r="A13" s="94">
         <v>3</v>
       </c>
       <c r="B13" s="38" t="s">
         <v>268</v>
       </c>
       <c r="C13" s="38"/>
-      <c r="D13" s="95" t="s">
+      <c r="D13" s="94" t="s">
         <v>267</v>
       </c>
-      <c r="E13" s="97">
+      <c r="E13" s="96">
         <v>2</v>
       </c>
       <c r="F13" s="38" t="s">
         <v>200</v>
       </c>
-      <c r="G13" s="95" t="s">
+      <c r="G13" s="94" t="s">
         <v>269</v>
       </c>
-      <c r="H13" s="95" t="s">
+      <c r="H13" s="94" t="s">
         <v>270</v>
       </c>
-      <c r="I13" s="95" t="s">
+      <c r="I13" s="94" t="s">
         <v>203</v>
       </c>
       <c r="J13" s="38">
@@ -6644,55 +6666,55 @@
         <v>10</v>
       </c>
       <c r="L13" s="38">
-        <f>J13+K13</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="M13" s="38">
-        <f>L13-E13</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="N13" s="38">
-        <f>(4*E13)-M13</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O13" s="38"/>
       <c r="P13" s="38"/>
       <c r="Q13" s="38"/>
       <c r="R13" s="39" t="e">
-        <f>Q13/P13</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="S13" s="95" t="s">
+      <c r="S13" s="94" t="s">
         <v>264</v>
       </c>
-      <c r="T13" s="95" t="s">
+      <c r="T13" s="94" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="14" spans="1:31" s="95" customFormat="1" ht="17" x14ac:dyDescent="0.15">
-      <c r="A14" s="95">
+    <row r="14" spans="1:31" s="94" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+      <c r="A14" s="94">
         <v>4</v>
       </c>
       <c r="B14" s="38" t="s">
         <v>271</v>
       </c>
       <c r="C14" s="38"/>
-      <c r="D14" s="95" t="s">
+      <c r="D14" s="94" t="s">
         <v>272</v>
       </c>
-      <c r="E14" s="97">
+      <c r="E14" s="96">
         <v>1</v>
       </c>
       <c r="F14" s="38" t="s">
         <v>200</v>
       </c>
-      <c r="G14" s="98" t="s">
+      <c r="G14" s="97" t="s">
         <v>432</v>
       </c>
-      <c r="H14" s="95" t="s">
+      <c r="H14" s="94" t="s">
         <v>273</v>
       </c>
-      <c r="I14" s="95" t="s">
+      <c r="I14" s="94" t="s">
         <v>203</v>
       </c>
       <c r="J14" s="38">
@@ -6703,15 +6725,15 @@
         <v>0</v>
       </c>
       <c r="L14" s="38">
-        <f>J14+K14</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="M14" s="38">
-        <f>L14-E14</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N14" s="38">
-        <f>(4*E14)-M14</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="O14" s="38"/>
@@ -6720,43 +6742,43 @@
       </c>
       <c r="Q14" s="38"/>
       <c r="R14" s="39">
-        <f>Q14/P14</f>
-        <v>0</v>
-      </c>
-      <c r="S14" s="95" t="s">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S14" s="94" t="s">
         <v>274</v>
       </c>
-      <c r="T14" s="95" t="s">
+      <c r="T14" s="94" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="15" spans="1:31" s="95" customFormat="1" ht="17" x14ac:dyDescent="0.15">
-      <c r="A15" s="95">
+    <row r="15" spans="1:31" s="94" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+      <c r="A15" s="94">
         <v>5</v>
       </c>
       <c r="B15" s="38" t="s">
         <v>276</v>
       </c>
       <c r="C15" s="38"/>
-      <c r="D15" s="95" t="s">
+      <c r="D15" s="94" t="s">
         <v>277</v>
       </c>
-      <c r="E15" s="97">
+      <c r="E15" s="96">
         <v>6</v>
       </c>
       <c r="F15" s="38" t="s">
         <v>200</v>
       </c>
-      <c r="G15" s="95" t="s">
+      <c r="G15" s="94" t="s">
         <v>278</v>
       </c>
-      <c r="H15" s="95" t="s">
+      <c r="H15" s="94" t="s">
         <v>103</v>
       </c>
-      <c r="I15" s="95" t="s">
+      <c r="I15" s="94" t="s">
         <v>203</v>
       </c>
-      <c r="J15" s="95">
+      <c r="J15" s="94">
         <v>4</v>
       </c>
       <c r="K15" s="38">
@@ -6764,15 +6786,15 @@
         <v>2</v>
       </c>
       <c r="L15" s="38">
-        <f>J15+K15</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="M15" s="38">
-        <f>L15-E15</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N15" s="38">
-        <f>(4*E15)-M15</f>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="O15" s="38"/>
@@ -6781,43 +6803,43 @@
       </c>
       <c r="Q15" s="41"/>
       <c r="R15" s="39">
-        <f>Q15/P15</f>
-        <v>0</v>
-      </c>
-      <c r="S15" s="95" t="s">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S15" s="94" t="s">
         <v>279</v>
       </c>
-      <c r="T15" s="95" t="s">
+      <c r="T15" s="94" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="16" spans="1:31" s="95" customFormat="1" ht="17" x14ac:dyDescent="0.15">
-      <c r="A16" s="95">
+    <row r="16" spans="1:31" s="94" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+      <c r="A16" s="94">
         <v>6</v>
       </c>
       <c r="B16" s="38" t="s">
         <v>281</v>
       </c>
       <c r="C16" s="38"/>
-      <c r="D16" s="95" t="s">
+      <c r="D16" s="94" t="s">
         <v>277</v>
       </c>
-      <c r="E16" s="97">
+      <c r="E16" s="96">
         <v>6</v>
       </c>
       <c r="F16" s="38" t="s">
         <v>200</v>
       </c>
-      <c r="G16" s="95" t="s">
+      <c r="G16" s="94" t="s">
         <v>282</v>
       </c>
       <c r="H16" s="38" t="s">
         <v>109</v>
       </c>
-      <c r="I16" s="95" t="s">
+      <c r="I16" s="94" t="s">
         <v>203</v>
       </c>
-      <c r="J16" s="95">
+      <c r="J16" s="94">
         <v>4</v>
       </c>
       <c r="K16" s="38">
@@ -6825,15 +6847,15 @@
         <v>2</v>
       </c>
       <c r="L16" s="38">
-        <f>J16+K16</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="M16" s="38">
-        <f>L16-E16</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N16" s="38">
-        <f>(4*E16)-M16</f>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="O16" s="38"/>
@@ -6842,43 +6864,43 @@
       </c>
       <c r="Q16" s="41"/>
       <c r="R16" s="39">
-        <f>Q16/P16</f>
-        <v>0</v>
-      </c>
-      <c r="S16" s="95" t="s">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S16" s="94" t="s">
         <v>283</v>
       </c>
-      <c r="T16" s="95" t="s">
+      <c r="T16" s="94" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="17" spans="1:31" s="95" customFormat="1" ht="17" x14ac:dyDescent="0.15">
-      <c r="A17" s="95">
+    <row r="17" spans="1:31" s="94" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+      <c r="A17" s="94">
         <v>7</v>
       </c>
       <c r="B17" s="38" t="s">
         <v>284</v>
       </c>
       <c r="C17" s="38"/>
-      <c r="D17" s="95" t="s">
+      <c r="D17" s="94" t="s">
         <v>285</v>
       </c>
-      <c r="E17" s="97">
+      <c r="E17" s="96">
         <v>1</v>
       </c>
       <c r="F17" s="38" t="s">
         <v>200</v>
       </c>
-      <c r="G17" s="95" t="s">
+      <c r="G17" s="94" t="s">
         <v>286</v>
       </c>
-      <c r="H17" s="95" t="s">
+      <c r="H17" s="94" t="s">
         <v>30</v>
       </c>
-      <c r="I17" s="95" t="s">
+      <c r="I17" s="94" t="s">
         <v>203</v>
       </c>
-      <c r="J17" s="95">
+      <c r="J17" s="94">
         <v>1</v>
       </c>
       <c r="K17" s="38">
@@ -6886,38 +6908,38 @@
         <v>0</v>
       </c>
       <c r="L17" s="38">
-        <f>J17+K17</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="M17" s="38">
-        <f>L17-E17</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N17" s="38">
-        <f>(4*E17)-M17</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="O17" s="38"/>
       <c r="P17" s="38"/>
       <c r="Q17" s="38"/>
       <c r="R17" s="39" t="e">
-        <f>Q17/P17</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="S17" s="95" t="s">
+      <c r="S17" s="94" t="s">
         <v>287</v>
       </c>
-      <c r="T17" s="95" t="s">
+      <c r="T17" s="94" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="18" spans="1:31" s="95" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="95">
+    <row r="18" spans="1:31" s="94" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="94">
         <v>8</v>
       </c>
       <c r="B18" s="38"/>
       <c r="C18" s="38"/>
-      <c r="E18" s="97"/>
+      <c r="E18" s="96"/>
       <c r="F18" s="38"/>
       <c r="K18" s="38"/>
       <c r="L18" s="38"/>
@@ -6927,20 +6949,20 @@
       <c r="P18" s="38"/>
       <c r="Q18" s="38"/>
       <c r="R18" s="39" t="e">
-        <f>Q18/P18</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="T18" s="95" t="s">
+      <c r="T18" s="94" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="19" spans="1:31" s="95" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="95">
+    <row r="19" spans="1:31" s="94" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="94">
         <v>9</v>
       </c>
       <c r="B19" s="38"/>
       <c r="C19" s="38"/>
-      <c r="E19" s="97"/>
+      <c r="E19" s="96"/>
       <c r="F19" s="38"/>
       <c r="K19" s="38"/>
       <c r="L19" s="38"/>
@@ -6950,40 +6972,40 @@
       <c r="P19" s="38"/>
       <c r="Q19" s="38"/>
       <c r="R19" s="39" t="e">
-        <f>Q19/P19</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="T19" s="95" t="s">
+      <c r="T19" s="94" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="20" spans="1:31" s="95" customFormat="1" ht="17" x14ac:dyDescent="0.15">
-      <c r="A20" s="95">
+    <row r="20" spans="1:31" s="94" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+      <c r="A20" s="94">
         <v>10</v>
       </c>
       <c r="B20" s="38" t="s">
         <v>288</v>
       </c>
       <c r="C20" s="38"/>
-      <c r="D20" s="95" t="s">
+      <c r="D20" s="94" t="s">
         <v>289</v>
       </c>
-      <c r="E20" s="97">
+      <c r="E20" s="96">
         <v>1</v>
       </c>
       <c r="F20" s="38" t="s">
         <v>200</v>
       </c>
-      <c r="G20" s="95" t="s">
+      <c r="G20" s="94" t="s">
         <v>290</v>
       </c>
-      <c r="H20" s="95" t="s">
+      <c r="H20" s="94" t="s">
         <v>291</v>
       </c>
-      <c r="I20" s="95" t="s">
+      <c r="I20" s="94" t="s">
         <v>203</v>
       </c>
-      <c r="J20" s="95">
+      <c r="J20" s="94">
         <v>1</v>
       </c>
       <c r="K20" s="38">
@@ -7006,55 +7028,55 @@
       <c r="P20" s="38"/>
       <c r="Q20" s="38"/>
       <c r="R20" s="39" t="e">
-        <f>Q20/P20</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="S20" s="95" t="s">
+      <c r="S20" s="94" t="s">
         <v>292</v>
       </c>
-      <c r="T20" s="95" t="s">
+      <c r="T20" s="94" t="s">
         <v>293</v>
       </c>
-      <c r="X20" s="95" t="s">
+      <c r="X20" s="94" t="s">
         <v>294</v>
       </c>
-      <c r="Z20" s="95">
+      <c r="Z20" s="94">
         <v>8.8000000000000007</v>
       </c>
-      <c r="AC20" s="95" t="s">
+      <c r="AC20" s="94" t="s">
         <v>295</v>
       </c>
-      <c r="AD20" s="95" t="s">
+      <c r="AD20" s="94" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="21" spans="1:31" s="95" customFormat="1" ht="17" x14ac:dyDescent="0.15">
-      <c r="A21" s="95">
+    <row r="21" spans="1:31" s="94" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+      <c r="A21" s="94">
         <v>11</v>
       </c>
       <c r="B21" s="38" t="s">
         <v>297</v>
       </c>
       <c r="C21" s="38"/>
-      <c r="D21" s="95" t="s">
+      <c r="D21" s="94" t="s">
         <v>298</v>
       </c>
-      <c r="E21" s="97">
+      <c r="E21" s="96">
         <v>1</v>
       </c>
       <c r="F21" s="38" t="s">
         <v>200</v>
       </c>
-      <c r="G21" s="95" t="s">
+      <c r="G21" s="94" t="s">
         <v>299</v>
       </c>
-      <c r="H21" s="95" t="s">
+      <c r="H21" s="94" t="s">
         <v>300</v>
       </c>
-      <c r="I21" s="95" t="s">
+      <c r="I21" s="94" t="s">
         <v>219</v>
       </c>
-      <c r="J21" s="95">
+      <c r="J21" s="94">
         <v>1</v>
       </c>
       <c r="K21" s="38">
@@ -7077,43 +7099,43 @@
       <c r="P21" s="38"/>
       <c r="Q21" s="38"/>
       <c r="R21" s="39" t="e">
-        <f>Q21/P21</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="S21" s="95" t="s">
+      <c r="S21" s="94" t="s">
         <v>301</v>
       </c>
-      <c r="T21" s="95" t="s">
+      <c r="T21" s="94" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="22" spans="1:31" s="95" customFormat="1" ht="17" x14ac:dyDescent="0.15">
-      <c r="A22" s="95">
+    <row r="22" spans="1:31" s="94" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+      <c r="A22" s="94">
         <v>12</v>
       </c>
       <c r="B22" s="38" t="s">
         <v>302</v>
       </c>
       <c r="C22" s="38"/>
-      <c r="D22" s="95" t="s">
+      <c r="D22" s="94" t="s">
         <v>303</v>
       </c>
-      <c r="E22" s="97">
+      <c r="E22" s="96">
         <v>4</v>
       </c>
       <c r="F22" s="38" t="s">
         <v>200</v>
       </c>
-      <c r="G22" s="95" t="s">
+      <c r="G22" s="94" t="s">
         <v>304</v>
       </c>
-      <c r="H22" s="95" t="s">
+      <c r="H22" s="94" t="s">
         <v>305</v>
       </c>
-      <c r="I22" s="95" t="s">
+      <c r="I22" s="94" t="s">
         <v>219</v>
       </c>
-      <c r="J22" s="95">
+      <c r="J22" s="94">
         <v>4</v>
       </c>
       <c r="K22" s="38">
@@ -7136,43 +7158,43 @@
       <c r="P22" s="38"/>
       <c r="Q22" s="38"/>
       <c r="R22" s="39" t="e">
-        <f>Q22/P22</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="S22" s="95" t="s">
+      <c r="S22" s="94" t="s">
         <v>306</v>
       </c>
-      <c r="T22" s="95" t="s">
+      <c r="T22" s="94" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="23" spans="1:31" s="95" customFormat="1" ht="17" x14ac:dyDescent="0.15">
-      <c r="A23" s="95">
+    <row r="23" spans="1:31" s="94" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+      <c r="A23" s="94">
         <v>13</v>
       </c>
       <c r="B23" s="38" t="s">
         <v>307</v>
       </c>
       <c r="C23" s="38"/>
-      <c r="D23" s="95" t="s">
+      <c r="D23" s="94" t="s">
         <v>308</v>
       </c>
-      <c r="E23" s="97">
+      <c r="E23" s="96">
         <v>1</v>
       </c>
       <c r="F23" s="38" t="s">
         <v>200</v>
       </c>
-      <c r="G23" s="96" t="s">
+      <c r="G23" s="95" t="s">
         <v>309</v>
       </c>
       <c r="H23" s="65" t="s">
         <v>310</v>
       </c>
-      <c r="I23" s="95" t="s">
+      <c r="I23" s="94" t="s">
         <v>219</v>
       </c>
-      <c r="J23" s="95">
+      <c r="J23" s="94">
         <v>0</v>
       </c>
       <c r="K23" s="38">
@@ -7195,43 +7217,43 @@
       <c r="P23" s="38"/>
       <c r="Q23" s="38"/>
       <c r="R23" s="39" t="e">
-        <f>Q23/P23</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="S23" s="95" t="s">
+      <c r="S23" s="94" t="s">
         <v>311</v>
       </c>
-      <c r="T23" s="95" t="s">
+      <c r="T23" s="94" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="24" spans="1:31" s="95" customFormat="1" ht="17" x14ac:dyDescent="0.15">
-      <c r="A24" s="95">
+    <row r="24" spans="1:31" s="94" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+      <c r="A24" s="94">
         <v>14</v>
       </c>
       <c r="B24" s="38" t="s">
         <v>312</v>
       </c>
       <c r="C24" s="38"/>
-      <c r="D24" s="95" t="s">
+      <c r="D24" s="94" t="s">
         <v>313</v>
       </c>
-      <c r="E24" s="97">
+      <c r="E24" s="96">
         <v>2</v>
       </c>
       <c r="F24" s="38" t="s">
         <v>200</v>
       </c>
-      <c r="G24" s="95" t="s">
+      <c r="G24" s="94" t="s">
         <v>314</v>
       </c>
-      <c r="H24" s="95" t="s">
+      <c r="H24" s="94" t="s">
         <v>315</v>
       </c>
-      <c r="I24" s="95" t="s">
+      <c r="I24" s="94" t="s">
         <v>203</v>
       </c>
-      <c r="J24" s="95">
+      <c r="J24" s="94">
         <v>2</v>
       </c>
       <c r="K24" s="38">
@@ -7254,23 +7276,23 @@
       <c r="P24" s="38"/>
       <c r="Q24" s="38"/>
       <c r="R24" s="39" t="e">
-        <f>Q24/P24</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="S24" s="95" t="s">
+      <c r="S24" s="94" t="s">
         <v>316</v>
       </c>
-      <c r="T24" s="95" t="s">
+      <c r="T24" s="94" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="25" spans="1:31" s="95" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="95">
+    <row r="25" spans="1:31" s="94" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="94">
         <v>15</v>
       </c>
       <c r="B25" s="38"/>
       <c r="C25" s="38"/>
-      <c r="E25" s="97"/>
+      <c r="E25" s="96"/>
       <c r="F25" s="38"/>
       <c r="K25" s="38"/>
       <c r="L25" s="38"/>
@@ -7280,17 +7302,17 @@
       <c r="P25" s="38"/>
       <c r="Q25" s="38"/>
       <c r="R25" s="39" t="e">
-        <f>Q25/P25</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="26" spans="1:31" s="95" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="95">
+    <row r="26" spans="1:31" s="94" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="94">
         <v>16</v>
       </c>
       <c r="B26" s="38"/>
       <c r="C26" s="38"/>
-      <c r="E26" s="97"/>
+      <c r="E26" s="96"/>
       <c r="F26" s="38"/>
       <c r="K26" s="38"/>
       <c r="L26" s="38"/>
@@ -7300,17 +7322,17 @@
       <c r="P26" s="38"/>
       <c r="Q26" s="38"/>
       <c r="R26" s="39" t="e">
-        <f>Q26/P26</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="27" spans="1:31" s="95" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="95">
+    <row r="27" spans="1:31" s="94" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="94">
         <v>17</v>
       </c>
       <c r="B27" s="38"/>
       <c r="C27" s="38"/>
-      <c r="E27" s="97"/>
+      <c r="E27" s="96"/>
       <c r="F27" s="38"/>
       <c r="K27" s="38"/>
       <c r="L27" s="38"/>
@@ -7320,17 +7342,17 @@
       <c r="P27" s="38"/>
       <c r="Q27" s="38"/>
       <c r="R27" s="39" t="e">
-        <f>Q27/P27</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="28" spans="1:31" s="95" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="95">
+    <row r="28" spans="1:31" s="94" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="94">
         <v>18</v>
       </c>
       <c r="B28" s="38"/>
       <c r="C28" s="38"/>
-      <c r="E28" s="97"/>
+      <c r="E28" s="96"/>
       <c r="F28" s="38"/>
       <c r="K28" s="38"/>
       <c r="L28" s="38"/>
@@ -7340,17 +7362,17 @@
       <c r="P28" s="38"/>
       <c r="Q28" s="38"/>
       <c r="R28" s="39" t="e">
-        <f>Q28/P28</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="29" spans="1:31" s="95" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="95">
+    <row r="29" spans="1:31" s="94" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="94">
         <v>19</v>
       </c>
       <c r="B29" s="38"/>
       <c r="C29" s="38"/>
-      <c r="E29" s="97"/>
+      <c r="E29" s="96"/>
       <c r="F29" s="38"/>
       <c r="K29" s="38"/>
       <c r="L29" s="38"/>
@@ -7361,13 +7383,13 @@
       <c r="Q29" s="38"/>
       <c r="R29" s="38"/>
     </row>
-    <row r="30" spans="1:31" s="95" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="95">
+    <row r="30" spans="1:31" s="94" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="94">
         <v>20</v>
       </c>
       <c r="B30" s="38"/>
       <c r="C30" s="38"/>
-      <c r="E30" s="97"/>
+      <c r="E30" s="96"/>
       <c r="F30" s="38"/>
       <c r="K30" s="38"/>
       <c r="L30" s="38"/>
@@ -7378,33 +7400,33 @@
       <c r="Q30" s="38"/>
       <c r="R30" s="38"/>
     </row>
-    <row r="31" spans="1:31" s="95" customFormat="1" ht="17" x14ac:dyDescent="0.15">
-      <c r="A31" s="95">
+    <row r="31" spans="1:31" s="94" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+      <c r="A31" s="94">
         <v>21</v>
       </c>
       <c r="B31" s="38" t="s">
         <v>317</v>
       </c>
       <c r="C31" s="38"/>
-      <c r="D31" s="95" t="s">
+      <c r="D31" s="94" t="s">
         <v>318</v>
       </c>
-      <c r="E31" s="97">
+      <c r="E31" s="96">
         <v>1</v>
       </c>
       <c r="F31" s="38" t="s">
         <v>200</v>
       </c>
-      <c r="G31" s="95" t="s">
+      <c r="G31" s="94" t="s">
         <v>319</v>
       </c>
-      <c r="H31" s="95" t="s">
+      <c r="H31" s="94" t="s">
         <v>320</v>
       </c>
-      <c r="I31" s="95" t="s">
+      <c r="I31" s="94" t="s">
         <v>203</v>
       </c>
-      <c r="J31" s="95">
+      <c r="J31" s="94">
         <v>1</v>
       </c>
       <c r="K31" s="38">
@@ -7412,210 +7434,210 @@
         <v>0</v>
       </c>
       <c r="L31" s="38">
-        <f>J31+K31</f>
+        <f t="shared" ref="L31:L55" si="4">J31+K31</f>
         <v>1</v>
       </c>
       <c r="M31" s="38">
-        <f>L31-E31</f>
+        <f t="shared" ref="M31:M55" si="5">L31-E31</f>
         <v>0</v>
       </c>
       <c r="N31" s="38">
-        <f>(4*E31)-M31</f>
+        <f t="shared" ref="N31:N55" si="6">(4*E31)-M31</f>
         <v>4</v>
       </c>
       <c r="O31" s="38"/>
       <c r="P31" s="38"/>
       <c r="Q31" s="38"/>
       <c r="R31" s="38"/>
-      <c r="S31" s="95" t="s">
+      <c r="S31" s="94" t="s">
         <v>321</v>
       </c>
-      <c r="T31" s="95" t="s">
+      <c r="T31" s="94" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="32" spans="1:31" s="95" customFormat="1" ht="17" x14ac:dyDescent="0.15">
-      <c r="A32" s="95">
+    <row r="32" spans="1:31" s="94" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+      <c r="A32" s="94">
         <v>22</v>
       </c>
       <c r="B32" s="38" t="s">
         <v>323</v>
       </c>
       <c r="C32" s="38"/>
-      <c r="D32" s="95" t="s">
+      <c r="D32" s="94" t="s">
         <v>318</v>
       </c>
-      <c r="E32" s="97">
+      <c r="E32" s="96">
         <v>10</v>
       </c>
       <c r="F32" s="38" t="s">
         <v>200</v>
       </c>
-      <c r="G32" s="95" t="s">
+      <c r="G32" s="94" t="s">
         <v>7</v>
       </c>
-      <c r="H32" s="95" t="s">
+      <c r="H32" s="94" t="s">
         <v>5</v>
       </c>
-      <c r="I32" s="95" t="s">
+      <c r="I32" s="94" t="s">
         <v>203</v>
       </c>
-      <c r="J32" s="95">
+      <c r="J32" s="94">
         <v>2</v>
       </c>
       <c r="K32" s="38">
         <v>10</v>
       </c>
       <c r="L32" s="38">
-        <f>J32+K32</f>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
       <c r="M32" s="38">
-        <f>L32-E32</f>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="N32" s="38">
-        <f>(4*E32)-M32</f>
+        <f t="shared" si="6"/>
         <v>38</v>
       </c>
       <c r="O32" s="38"/>
       <c r="P32" s="38"/>
       <c r="Q32" s="38"/>
       <c r="R32" s="38"/>
-      <c r="S32" s="95" t="s">
+      <c r="S32" s="94" t="s">
         <v>324</v>
       </c>
-      <c r="T32" s="95" t="s">
+      <c r="T32" s="94" t="s">
         <v>325</v>
       </c>
-      <c r="U32" s="95" t="s">
+      <c r="U32" s="94" t="s">
         <v>326</v>
       </c>
-      <c r="V32" s="95" t="s">
+      <c r="V32" s="94" t="s">
         <v>325</v>
       </c>
-      <c r="W32" s="95" t="s">
+      <c r="W32" s="94" t="s">
         <v>327</v>
       </c>
-      <c r="X32" s="95" t="s">
+      <c r="X32" s="94" t="s">
         <v>8</v>
       </c>
-      <c r="Y32" s="95" t="s">
+      <c r="Y32" s="94" t="s">
         <v>328</v>
       </c>
-      <c r="AA32" s="95" t="s">
+      <c r="AA32" s="94" t="s">
         <v>7</v>
       </c>
-      <c r="AB32" s="95" t="s">
+      <c r="AB32" s="94" t="s">
         <v>329</v>
       </c>
-      <c r="AE32" s="95" t="s">
+      <c r="AE32" s="94" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="33" spans="1:31" s="95" customFormat="1" ht="34" x14ac:dyDescent="0.15">
-      <c r="A33" s="95">
+    <row r="33" spans="1:31" s="94" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+      <c r="A33" s="94">
         <v>23</v>
       </c>
       <c r="B33" s="38" t="s">
         <v>331</v>
       </c>
       <c r="C33" s="38"/>
-      <c r="D33" s="95" t="s">
+      <c r="D33" s="94" t="s">
         <v>318</v>
       </c>
-      <c r="E33" s="97">
+      <c r="E33" s="96">
         <v>11</v>
       </c>
       <c r="F33" s="38" t="s">
         <v>200</v>
       </c>
-      <c r="G33" s="95" t="s">
+      <c r="G33" s="94" t="s">
         <v>13</v>
       </c>
-      <c r="H33" s="95" t="s">
+      <c r="H33" s="94" t="s">
         <v>12</v>
       </c>
-      <c r="I33" s="95" t="s">
+      <c r="I33" s="94" t="s">
         <v>203</v>
       </c>
-      <c r="J33" s="95">
+      <c r="J33" s="94">
         <v>2</v>
       </c>
       <c r="K33" s="38">
         <v>10</v>
       </c>
       <c r="L33" s="38">
-        <f>J33+K33</f>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
       <c r="M33" s="38">
-        <f>L33-E33</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="N33" s="38">
-        <f>(4*E33)-M33</f>
+        <f t="shared" si="6"/>
         <v>43</v>
       </c>
       <c r="O33" s="38"/>
       <c r="P33" s="38"/>
       <c r="Q33" s="38"/>
       <c r="R33" s="38"/>
-      <c r="S33" s="95" t="s">
+      <c r="S33" s="94" t="s">
         <v>332</v>
       </c>
-      <c r="T33" s="95" t="s">
+      <c r="T33" s="94" t="s">
         <v>333</v>
       </c>
-      <c r="U33" s="95" t="s">
+      <c r="U33" s="94" t="s">
         <v>326</v>
       </c>
-      <c r="V33" s="95" t="s">
+      <c r="V33" s="94" t="s">
         <v>333</v>
       </c>
-      <c r="W33" s="95" t="s">
+      <c r="W33" s="94" t="s">
         <v>334</v>
       </c>
-      <c r="X33" s="95" t="s">
+      <c r="X33" s="94" t="s">
         <v>14</v>
       </c>
-      <c r="Y33" s="95" t="s">
+      <c r="Y33" s="94" t="s">
         <v>328</v>
       </c>
-      <c r="AA33" s="95" t="s">
+      <c r="AA33" s="94" t="s">
         <v>13</v>
       </c>
-      <c r="AB33" s="95" t="s">
+      <c r="AB33" s="94" t="s">
         <v>329</v>
       </c>
-      <c r="AE33" s="95" t="s">
+      <c r="AE33" s="94" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="34" spans="1:31" s="95" customFormat="1" ht="17" x14ac:dyDescent="0.15">
-      <c r="A34" s="95">
+    <row r="34" spans="1:31" s="94" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+      <c r="A34" s="94">
         <v>24</v>
       </c>
       <c r="B34" s="38" t="s">
         <v>335</v>
       </c>
       <c r="C34" s="38"/>
-      <c r="D34" s="95" t="s">
+      <c r="D34" s="94" t="s">
         <v>336</v>
       </c>
-      <c r="E34" s="97">
+      <c r="E34" s="96">
         <v>1</v>
       </c>
       <c r="F34" s="38" t="s">
         <v>200</v>
       </c>
-      <c r="G34" s="95">
+      <c r="G34" s="94">
         <v>0.1</v>
       </c>
-      <c r="I34" s="95" t="s">
+      <c r="I34" s="94" t="s">
         <v>203</v>
       </c>
-      <c r="J34" s="95">
+      <c r="J34" s="94">
         <v>1</v>
       </c>
       <c r="K34" s="38">
@@ -7623,273 +7645,273 @@
         <v>0</v>
       </c>
       <c r="L34" s="38">
-        <f>J34+K34</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="M34" s="38">
-        <f>L34-E34</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N34" s="38">
-        <f>(4*E34)-M34</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="O34" s="38"/>
       <c r="P34" s="38"/>
       <c r="Q34" s="38"/>
       <c r="R34" s="38"/>
-      <c r="S34" s="95" t="s">
+      <c r="S34" s="94" t="s">
         <v>337</v>
       </c>
-      <c r="T34" s="95" t="s">
+      <c r="T34" s="94" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="35" spans="1:31" s="95" customFormat="1" ht="17" x14ac:dyDescent="0.15">
-      <c r="A35" s="95">
+    <row r="35" spans="1:31" s="94" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+      <c r="A35" s="94">
         <v>25</v>
       </c>
       <c r="B35" s="38" t="s">
         <v>338</v>
       </c>
       <c r="C35" s="38"/>
-      <c r="D35" s="95" t="s">
+      <c r="D35" s="94" t="s">
         <v>336</v>
       </c>
-      <c r="E35" s="97">
+      <c r="E35" s="96">
         <v>2</v>
       </c>
       <c r="F35" s="38" t="s">
         <v>200</v>
       </c>
-      <c r="G35" s="95" t="s">
+      <c r="G35" s="94" t="s">
         <v>221</v>
       </c>
-      <c r="H35" s="95" t="s">
+      <c r="H35" s="94" t="s">
         <v>97</v>
       </c>
-      <c r="I35" s="95" t="s">
+      <c r="I35" s="94" t="s">
         <v>203</v>
       </c>
-      <c r="J35" s="95">
+      <c r="J35" s="94">
         <v>0</v>
       </c>
       <c r="K35" s="38">
         <v>10</v>
       </c>
       <c r="L35" s="38">
-        <f>J35+K35</f>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="M35" s="38">
-        <f>L35-E35</f>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="N35" s="38">
-        <f>(4*E35)-M35</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="O35" s="38"/>
       <c r="P35" s="38"/>
       <c r="Q35" s="38"/>
       <c r="R35" s="38"/>
-      <c r="S35" s="95" t="s">
+      <c r="S35" s="94" t="s">
         <v>337</v>
       </c>
-      <c r="T35" s="95" t="s">
+      <c r="T35" s="94" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="36" spans="1:31" s="95" customFormat="1" ht="17" x14ac:dyDescent="0.15">
-      <c r="A36" s="95">
+    <row r="36" spans="1:31" s="94" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+      <c r="A36" s="94">
         <v>26</v>
       </c>
       <c r="B36" s="38" t="s">
         <v>339</v>
       </c>
       <c r="C36" s="38"/>
-      <c r="D36" s="95" t="s">
+      <c r="D36" s="94" t="s">
         <v>336</v>
       </c>
-      <c r="E36" s="97">
+      <c r="E36" s="96">
         <v>1</v>
       </c>
       <c r="F36" s="38" t="s">
         <v>200</v>
       </c>
-      <c r="G36" s="95">
+      <c r="G36" s="94">
         <v>300</v>
       </c>
-      <c r="H36" s="95" t="s">
+      <c r="H36" s="94" t="s">
         <v>340</v>
       </c>
-      <c r="I36" s="95" t="s">
+      <c r="I36" s="94" t="s">
         <v>203</v>
       </c>
-      <c r="J36" s="95">
+      <c r="J36" s="94">
         <v>0</v>
       </c>
       <c r="K36" s="38"/>
       <c r="L36" s="38">
-        <f>J36+K36</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="M36" s="38">
-        <f>L36-E36</f>
+        <f t="shared" si="5"/>
         <v>-1</v>
       </c>
       <c r="N36" s="38">
-        <f>(4*E36)-M36</f>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="O36" s="38"/>
       <c r="P36" s="38"/>
       <c r="Q36" s="38"/>
       <c r="R36" s="38"/>
-      <c r="S36" s="95" t="s">
+      <c r="S36" s="94" t="s">
         <v>337</v>
       </c>
-      <c r="T36" s="95" t="s">
+      <c r="T36" s="94" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="37" spans="1:31" s="95" customFormat="1" ht="51" x14ac:dyDescent="0.15">
-      <c r="A37" s="95">
+    <row r="37" spans="1:31" s="94" customFormat="1" ht="51" x14ac:dyDescent="0.15">
+      <c r="A37" s="94">
         <v>27</v>
       </c>
       <c r="B37" s="38" t="s">
         <v>341</v>
       </c>
       <c r="C37" s="38"/>
-      <c r="D37" s="95" t="s">
+      <c r="D37" s="94" t="s">
         <v>336</v>
       </c>
-      <c r="E37" s="97">
+      <c r="E37" s="96">
         <v>21</v>
       </c>
       <c r="F37" s="38" t="s">
         <v>200</v>
       </c>
-      <c r="G37" s="95">
+      <c r="G37" s="94">
         <v>470</v>
       </c>
-      <c r="H37" s="95" t="s">
+      <c r="H37" s="94" t="s">
         <v>342</v>
       </c>
-      <c r="I37" s="95" t="s">
+      <c r="I37" s="94" t="s">
         <v>203</v>
       </c>
-      <c r="J37" s="95">
+      <c r="J37" s="94">
         <v>11</v>
       </c>
       <c r="K37" s="38">
         <v>20</v>
       </c>
       <c r="L37" s="38">
-        <f>J37+K37</f>
+        <f t="shared" si="4"/>
         <v>31</v>
       </c>
       <c r="M37" s="38">
-        <f>L37-E37</f>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="N37" s="38">
-        <f>(4*E37)-M37</f>
+        <f t="shared" si="6"/>
         <v>74</v>
       </c>
       <c r="O37" s="38"/>
       <c r="P37" s="38"/>
       <c r="Q37" s="38"/>
       <c r="R37" s="38"/>
-      <c r="S37" s="95" t="s">
+      <c r="S37" s="94" t="s">
         <v>337</v>
       </c>
-      <c r="T37" s="95" t="s">
+      <c r="T37" s="94" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="38" spans="1:31" s="95" customFormat="1" ht="17" x14ac:dyDescent="0.15">
-      <c r="A38" s="95">
+    <row r="38" spans="1:31" s="94" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+      <c r="A38" s="94">
         <v>28</v>
       </c>
       <c r="B38" s="38" t="s">
         <v>343</v>
       </c>
       <c r="C38" s="38"/>
-      <c r="D38" s="95" t="s">
+      <c r="D38" s="94" t="s">
         <v>336</v>
       </c>
-      <c r="E38" s="97">
+      <c r="E38" s="96">
         <v>6</v>
       </c>
       <c r="F38" s="38" t="s">
         <v>200</v>
       </c>
-      <c r="G38" s="95" t="s">
+      <c r="G38" s="94" t="s">
         <v>344</v>
       </c>
-      <c r="H38" s="95" t="s">
+      <c r="H38" s="94" t="s">
         <v>65</v>
       </c>
-      <c r="I38" s="95" t="s">
+      <c r="I38" s="94" t="s">
         <v>203</v>
       </c>
-      <c r="J38" s="95">
+      <c r="J38" s="94">
         <v>4</v>
       </c>
       <c r="K38" s="38">
         <v>10</v>
       </c>
       <c r="L38" s="38">
-        <f>J38+K38</f>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="M38" s="38">
-        <f>L38-E38</f>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="N38" s="38">
-        <f>(4*E38)-M38</f>
+        <f t="shared" si="6"/>
         <v>16</v>
       </c>
       <c r="O38" s="38"/>
       <c r="P38" s="38"/>
       <c r="Q38" s="38"/>
       <c r="R38" s="38"/>
-      <c r="S38" s="95" t="s">
+      <c r="S38" s="94" t="s">
         <v>337</v>
       </c>
-      <c r="T38" s="95" t="s">
+      <c r="T38" s="94" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="39" spans="1:31" s="95" customFormat="1" ht="17" x14ac:dyDescent="0.15">
-      <c r="A39" s="95">
+    <row r="39" spans="1:31" s="94" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+      <c r="A39" s="94">
         <v>29</v>
       </c>
       <c r="B39" s="38" t="s">
         <v>345</v>
       </c>
       <c r="C39" s="38"/>
-      <c r="D39" s="95" t="s">
+      <c r="D39" s="94" t="s">
         <v>336</v>
       </c>
-      <c r="E39" s="97">
+      <c r="E39" s="96">
         <v>3</v>
       </c>
       <c r="F39" s="38" t="s">
         <v>200</v>
       </c>
-      <c r="G39" s="95" t="s">
+      <c r="G39" s="94" t="s">
         <v>346</v>
       </c>
-      <c r="H39" s="95" t="s">
+      <c r="H39" s="94" t="s">
         <v>89</v>
       </c>
-      <c r="I39" s="95" t="s">
+      <c r="I39" s="94" t="s">
         <v>203</v>
       </c>
-      <c r="J39" s="95">
+      <c r="J39" s="94">
         <v>8</v>
       </c>
       <c r="K39" s="38">
@@ -7897,55 +7919,55 @@
         <v>0</v>
       </c>
       <c r="L39" s="38">
-        <f>J39+K39</f>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="M39" s="38">
-        <f>L39-E39</f>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="N39" s="38">
-        <f>(4*E39)-M39</f>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="O39" s="38"/>
       <c r="P39" s="38"/>
       <c r="Q39" s="38"/>
       <c r="R39" s="38"/>
-      <c r="S39" s="95" t="s">
+      <c r="S39" s="94" t="s">
         <v>337</v>
       </c>
-      <c r="T39" s="95" t="s">
+      <c r="T39" s="94" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="40" spans="1:31" s="95" customFormat="1" ht="17" x14ac:dyDescent="0.15">
-      <c r="A40" s="95">
+    <row r="40" spans="1:31" s="94" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+      <c r="A40" s="94">
         <v>30</v>
       </c>
       <c r="B40" s="38" t="s">
         <v>347</v>
       </c>
       <c r="C40" s="38"/>
-      <c r="D40" s="95" t="s">
+      <c r="D40" s="94" t="s">
         <v>336</v>
       </c>
-      <c r="E40" s="97">
+      <c r="E40" s="96">
         <v>2</v>
       </c>
       <c r="F40" s="38" t="s">
         <v>200</v>
       </c>
-      <c r="G40" s="95" t="s">
+      <c r="G40" s="94" t="s">
         <v>348</v>
       </c>
-      <c r="H40" s="95" t="s">
+      <c r="H40" s="94" t="s">
         <v>94</v>
       </c>
-      <c r="I40" s="95" t="s">
+      <c r="I40" s="94" t="s">
         <v>203</v>
       </c>
-      <c r="J40" s="95">
+      <c r="J40" s="94">
         <v>8</v>
       </c>
       <c r="K40" s="38">
@@ -7953,786 +7975,786 @@
         <v>0</v>
       </c>
       <c r="L40" s="38">
-        <f>J40+K40</f>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="M40" s="38">
-        <f>L40-E40</f>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="N40" s="38">
-        <f>(4*E40)-M40</f>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="O40" s="38"/>
       <c r="P40" s="38"/>
       <c r="Q40" s="38"/>
       <c r="R40" s="38"/>
-      <c r="S40" s="95" t="s">
+      <c r="S40" s="94" t="s">
         <v>337</v>
       </c>
-      <c r="T40" s="95" t="s">
+      <c r="T40" s="94" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="41" spans="1:31" s="95" customFormat="1" ht="17" x14ac:dyDescent="0.15">
-      <c r="A41" s="95">
+    <row r="41" spans="1:31" s="94" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+      <c r="A41" s="94">
         <v>31</v>
       </c>
       <c r="B41" s="38" t="s">
         <v>349</v>
       </c>
       <c r="C41" s="38"/>
-      <c r="D41" s="95" t="s">
+      <c r="D41" s="94" t="s">
         <v>336</v>
       </c>
-      <c r="E41" s="97">
+      <c r="E41" s="96">
         <v>2</v>
       </c>
       <c r="F41" s="38" t="s">
         <v>200</v>
       </c>
-      <c r="G41" s="95">
+      <c r="G41" s="94">
         <v>11</v>
       </c>
-      <c r="H41" s="95" t="s">
+      <c r="H41" s="94" t="s">
         <v>350</v>
       </c>
-      <c r="I41" s="95" t="s">
+      <c r="I41" s="94" t="s">
         <v>203</v>
       </c>
-      <c r="J41" s="95">
+      <c r="J41" s="94">
         <v>0</v>
       </c>
       <c r="K41" s="38">
         <v>10</v>
       </c>
       <c r="L41" s="38">
-        <f>J41+K41</f>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="M41" s="38">
-        <f>L41-E41</f>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="N41" s="38">
-        <f>(4*E41)-M41</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="O41" s="38"/>
       <c r="P41" s="38"/>
       <c r="Q41" s="38"/>
       <c r="R41" s="38"/>
-      <c r="S41" s="95" t="s">
+      <c r="S41" s="94" t="s">
         <v>337</v>
       </c>
-      <c r="T41" s="95" t="s">
+      <c r="T41" s="94" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="42" spans="1:31" s="95" customFormat="1" ht="17" x14ac:dyDescent="0.15">
-      <c r="A42" s="95">
+    <row r="42" spans="1:31" s="94" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+      <c r="A42" s="94">
         <v>32</v>
       </c>
       <c r="B42" s="38" t="s">
         <v>351</v>
       </c>
       <c r="C42" s="38"/>
-      <c r="D42" s="95" t="s">
+      <c r="D42" s="94" t="s">
         <v>336</v>
       </c>
-      <c r="E42" s="97">
+      <c r="E42" s="96">
         <v>6</v>
       </c>
       <c r="F42" s="38" t="s">
         <v>200</v>
       </c>
-      <c r="G42" s="95" t="s">
+      <c r="G42" s="94" t="s">
         <v>352</v>
       </c>
-      <c r="H42" s="95" t="s">
+      <c r="H42" s="94" t="s">
         <v>82</v>
       </c>
-      <c r="I42" s="95" t="s">
+      <c r="I42" s="94" t="s">
         <v>203</v>
       </c>
-      <c r="J42" s="95">
+      <c r="J42" s="94">
         <v>6</v>
       </c>
       <c r="K42" s="38">
-        <f>IF(J42&gt;E42,0,E42-J42)</f>
+        <f t="shared" ref="K42:K55" si="7">IF(J42&gt;E42,0,E42-J42)</f>
         <v>0</v>
       </c>
       <c r="L42" s="38">
-        <f>J42+K42</f>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="M42" s="38">
-        <f>L42-E42</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N42" s="38">
-        <f>(4*E42)-M42</f>
+        <f t="shared" si="6"/>
         <v>24</v>
       </c>
       <c r="O42" s="38"/>
       <c r="P42" s="38"/>
       <c r="Q42" s="38"/>
       <c r="R42" s="38"/>
-      <c r="S42" s="95" t="s">
+      <c r="S42" s="94" t="s">
         <v>337</v>
       </c>
-      <c r="T42" s="95" t="s">
+      <c r="T42" s="94" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="43" spans="1:31" s="95" customFormat="1" ht="17" x14ac:dyDescent="0.15">
-      <c r="A43" s="95">
+    <row r="43" spans="1:31" s="94" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+      <c r="A43" s="94">
         <v>33</v>
       </c>
       <c r="B43" s="38" t="s">
         <v>353</v>
       </c>
       <c r="C43" s="38"/>
-      <c r="D43" s="95" t="s">
+      <c r="D43" s="94" t="s">
         <v>354</v>
       </c>
-      <c r="E43" s="97">
+      <c r="E43" s="96">
         <v>1</v>
       </c>
       <c r="F43" s="38" t="s">
         <v>200</v>
       </c>
-      <c r="G43" s="95" t="s">
+      <c r="G43" s="94" t="s">
         <v>355</v>
       </c>
-      <c r="H43" s="95" t="s">
+      <c r="H43" s="94" t="s">
         <v>356</v>
       </c>
-      <c r="I43" s="95" t="s">
+      <c r="I43" s="94" t="s">
         <v>203</v>
       </c>
-      <c r="J43" s="95">
+      <c r="J43" s="94">
         <v>1</v>
       </c>
       <c r="K43" s="38">
-        <f>IF(J43&gt;E43,0,E43-J43)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L43" s="38">
-        <f>J43+K43</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="M43" s="38">
-        <f>L43-E43</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N43" s="38">
-        <f>(4*E43)-M43</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="O43" s="38"/>
       <c r="P43" s="38"/>
       <c r="Q43" s="38"/>
       <c r="R43" s="38"/>
-      <c r="S43" s="95" t="s">
+      <c r="S43" s="94" t="s">
         <v>357</v>
       </c>
-      <c r="T43" s="95" t="s">
+      <c r="T43" s="94" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="44" spans="1:31" s="95" customFormat="1" ht="17" x14ac:dyDescent="0.15">
-      <c r="A44" s="95">
+    <row r="44" spans="1:31" s="94" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+      <c r="A44" s="94">
         <v>34</v>
       </c>
       <c r="B44" s="38" t="s">
         <v>222</v>
       </c>
       <c r="C44" s="38"/>
-      <c r="D44" s="95" t="s">
+      <c r="D44" s="94" t="s">
         <v>358</v>
       </c>
-      <c r="E44" s="97">
+      <c r="E44" s="96">
         <v>1</v>
       </c>
       <c r="F44" s="38" t="s">
         <v>200</v>
       </c>
-      <c r="G44" s="95" t="s">
+      <c r="G44" s="94" t="s">
         <v>359</v>
       </c>
-      <c r="H44" s="95" t="s">
+      <c r="H44" s="94" t="s">
         <v>360</v>
       </c>
-      <c r="I44" s="95" t="s">
+      <c r="I44" s="94" t="s">
         <v>203</v>
       </c>
-      <c r="J44" s="95">
+      <c r="J44" s="94">
         <v>1</v>
       </c>
       <c r="K44" s="38">
-        <f>IF(J44&gt;E44,0,E44-J44)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L44" s="38">
-        <f>J44+K44</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="M44" s="38">
-        <f>L44-E44</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N44" s="38">
-        <f>(4*E44)-M44</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="O44" s="38"/>
       <c r="P44" s="38"/>
       <c r="Q44" s="38"/>
       <c r="R44" s="38"/>
-      <c r="S44" s="95" t="s">
+      <c r="S44" s="94" t="s">
         <v>361</v>
       </c>
-      <c r="T44" s="95" t="s">
+      <c r="T44" s="94" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="45" spans="1:31" s="95" customFormat="1" ht="17" x14ac:dyDescent="0.15">
-      <c r="A45" s="95">
+    <row r="45" spans="1:31" s="94" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+      <c r="A45" s="94">
         <v>35</v>
       </c>
       <c r="B45" s="38" t="s">
         <v>363</v>
       </c>
       <c r="C45" s="38"/>
-      <c r="D45" s="95" t="s">
+      <c r="D45" s="94" t="s">
         <v>364</v>
       </c>
-      <c r="E45" s="97">
+      <c r="E45" s="96">
         <v>1</v>
       </c>
       <c r="F45" s="38" t="s">
         <v>200</v>
       </c>
-      <c r="G45" s="95" t="s">
+      <c r="G45" s="94" t="s">
         <v>137</v>
       </c>
-      <c r="I45" s="95" t="s">
+      <c r="I45" s="94" t="s">
         <v>203</v>
       </c>
-      <c r="J45" s="95">
+      <c r="J45" s="94">
         <v>1</v>
       </c>
       <c r="K45" s="38">
-        <f>IF(J45&gt;E45,0,E45-J45)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L45" s="38">
-        <f>J45+K45</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="M45" s="38">
-        <f>L45-E45</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N45" s="38">
-        <f>(4*E45)-M45</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="O45" s="38"/>
       <c r="P45" s="38"/>
       <c r="Q45" s="38"/>
       <c r="R45" s="38"/>
-      <c r="S45" s="95" t="s">
+      <c r="S45" s="94" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="46" spans="1:31" s="95" customFormat="1" ht="17" x14ac:dyDescent="0.15">
-      <c r="A46" s="95">
+    <row r="46" spans="1:31" s="94" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+      <c r="A46" s="94">
         <v>36</v>
       </c>
       <c r="B46" s="38" t="s">
         <v>223</v>
       </c>
       <c r="C46" s="38"/>
-      <c r="D46" s="95" t="s">
+      <c r="D46" s="94" t="s">
         <v>366</v>
       </c>
-      <c r="E46" s="97">
+      <c r="E46" s="96">
         <v>1</v>
       </c>
       <c r="F46" s="38" t="s">
         <v>200</v>
       </c>
-      <c r="G46" s="95" t="s">
+      <c r="G46" s="94" t="s">
         <v>367</v>
       </c>
-      <c r="H46" s="95" t="s">
+      <c r="H46" s="94" t="s">
         <v>368</v>
       </c>
-      <c r="I46" s="95" t="s">
+      <c r="I46" s="94" t="s">
         <v>203</v>
       </c>
-      <c r="J46" s="95">
+      <c r="J46" s="94">
         <v>0</v>
       </c>
       <c r="K46" s="38">
-        <f>IF(J46&gt;E46,0,E46-J46)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="L46" s="38">
-        <f>J46+K46</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="M46" s="38">
-        <f>L46-E46</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N46" s="38">
-        <f>(4*E46)-M46</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="O46" s="38"/>
       <c r="P46" s="38"/>
       <c r="Q46" s="38"/>
       <c r="R46" s="38"/>
-      <c r="S46" s="95" t="s">
+      <c r="S46" s="94" t="s">
         <v>369</v>
       </c>
-      <c r="T46" s="95" t="s">
+      <c r="T46" s="94" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="47" spans="1:31" s="95" customFormat="1" ht="17" x14ac:dyDescent="0.15">
-      <c r="A47" s="95">
+    <row r="47" spans="1:31" s="94" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+      <c r="A47" s="94">
         <v>37</v>
       </c>
       <c r="B47" s="38" t="s">
         <v>371</v>
       </c>
       <c r="C47" s="38"/>
-      <c r="D47" s="95" t="s">
+      <c r="D47" s="94" t="s">
         <v>372</v>
       </c>
-      <c r="E47" s="97">
+      <c r="E47" s="96">
         <v>1</v>
       </c>
       <c r="F47" s="38" t="s">
         <v>200</v>
       </c>
-      <c r="G47" s="95" t="s">
+      <c r="G47" s="94" t="s">
         <v>373</v>
       </c>
-      <c r="H47" s="95" t="s">
+      <c r="H47" s="94" t="s">
         <v>374</v>
       </c>
-      <c r="I47" s="95" t="s">
+      <c r="I47" s="94" t="s">
         <v>203</v>
       </c>
-      <c r="J47" s="95">
+      <c r="J47" s="94">
         <v>1</v>
       </c>
       <c r="K47" s="38">
-        <f>IF(J47&gt;E47,0,E47-J47)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L47" s="38">
-        <f>J47+K47</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="M47" s="38">
-        <f>L47-E47</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N47" s="38">
-        <f>(4*E47)-M47</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="O47" s="38"/>
       <c r="P47" s="38"/>
       <c r="Q47" s="38"/>
       <c r="R47" s="38"/>
-      <c r="S47" s="95" t="s">
+      <c r="S47" s="94" t="s">
         <v>375</v>
       </c>
-      <c r="T47" s="95" t="s">
+      <c r="T47" s="94" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="48" spans="1:31" s="95" customFormat="1" ht="17" x14ac:dyDescent="0.15">
-      <c r="A48" s="95">
+    <row r="48" spans="1:31" s="94" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+      <c r="A48" s="94">
         <v>38</v>
       </c>
       <c r="B48" s="38" t="s">
         <v>377</v>
       </c>
       <c r="C48" s="38"/>
-      <c r="D48" s="95" t="s">
+      <c r="D48" s="94" t="s">
         <v>378</v>
       </c>
-      <c r="E48" s="97">
+      <c r="E48" s="96">
         <v>2</v>
       </c>
       <c r="F48" s="38" t="s">
         <v>200</v>
       </c>
-      <c r="G48" s="95" t="s">
+      <c r="G48" s="94" t="s">
         <v>379</v>
       </c>
-      <c r="H48" s="95" t="s">
+      <c r="H48" s="94" t="s">
         <v>380</v>
       </c>
-      <c r="I48" s="95" t="s">
+      <c r="I48" s="94" t="s">
         <v>203</v>
       </c>
-      <c r="J48" s="95">
+      <c r="J48" s="94">
         <v>2</v>
       </c>
       <c r="K48" s="38">
-        <f>IF(J48&gt;E48,0,E48-J48)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L48" s="38">
-        <f>J48+K48</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="M48" s="38">
-        <f>L48-E48</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N48" s="38">
-        <f>(4*E48)-M48</f>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="O48" s="38"/>
       <c r="P48" s="38"/>
       <c r="Q48" s="38"/>
       <c r="R48" s="38"/>
-      <c r="S48" s="95" t="s">
+      <c r="S48" s="94" t="s">
         <v>381</v>
       </c>
-      <c r="T48" s="95" t="s">
+      <c r="T48" s="94" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="49" spans="1:20" s="95" customFormat="1" ht="17" x14ac:dyDescent="0.15">
-      <c r="A49" s="95">
+    <row r="49" spans="1:20" s="94" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+      <c r="A49" s="94">
         <v>39</v>
       </c>
       <c r="B49" s="38" t="s">
         <v>227</v>
       </c>
       <c r="C49" s="38"/>
-      <c r="D49" s="95" t="s">
+      <c r="D49" s="94" t="s">
         <v>383</v>
       </c>
-      <c r="E49" s="97">
+      <c r="E49" s="96">
         <v>1</v>
       </c>
       <c r="F49" s="38" t="s">
         <v>200</v>
       </c>
-      <c r="G49" s="95" t="s">
+      <c r="G49" s="94" t="s">
         <v>384</v>
       </c>
-      <c r="H49" s="95" t="s">
+      <c r="H49" s="94" t="s">
         <v>17</v>
       </c>
-      <c r="I49" s="95" t="s">
+      <c r="I49" s="94" t="s">
         <v>203</v>
       </c>
-      <c r="J49" s="95">
+      <c r="J49" s="94">
         <v>1</v>
       </c>
       <c r="K49" s="38">
-        <f>IF(J49&gt;E49,0,E49-J49)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L49" s="38">
-        <f>J49+K49</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="M49" s="38">
-        <f>L49-E49</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N49" s="38">
-        <f>(4*E49)-M49</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="O49" s="38"/>
       <c r="P49" s="38"/>
       <c r="Q49" s="38"/>
       <c r="R49" s="38"/>
-      <c r="S49" s="95" t="s">
+      <c r="S49" s="94" t="s">
         <v>385</v>
       </c>
-      <c r="T49" s="95" t="s">
+      <c r="T49" s="94" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="50" spans="1:20" s="95" customFormat="1" ht="17" x14ac:dyDescent="0.15">
-      <c r="A50" s="95">
+    <row r="50" spans="1:20" s="94" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+      <c r="A50" s="94">
         <v>40</v>
       </c>
       <c r="B50" s="38" t="s">
         <v>229</v>
       </c>
       <c r="C50" s="38"/>
-      <c r="D50" s="95" t="s">
+      <c r="D50" s="94" t="s">
         <v>387</v>
       </c>
-      <c r="E50" s="97">
+      <c r="E50" s="96">
         <v>1</v>
       </c>
       <c r="F50" s="38" t="s">
         <v>200</v>
       </c>
-      <c r="G50" s="95" t="s">
+      <c r="G50" s="94" t="s">
         <v>388</v>
       </c>
-      <c r="H50" s="95" t="s">
+      <c r="H50" s="94" t="s">
         <v>389</v>
       </c>
-      <c r="I50" s="95" t="s">
+      <c r="I50" s="94" t="s">
         <v>203</v>
       </c>
-      <c r="J50" s="95">
+      <c r="J50" s="94">
         <v>1</v>
       </c>
       <c r="K50" s="38">
-        <f>IF(J50&gt;E50,0,E50-J50)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L50" s="38">
-        <f>J50+K50</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="M50" s="38">
-        <f>L50-E50</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N50" s="38">
-        <f>(4*E50)-M50</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="O50" s="38"/>
       <c r="P50" s="38"/>
       <c r="Q50" s="38"/>
       <c r="R50" s="38"/>
-      <c r="S50" s="95" t="s">
+      <c r="S50" s="94" t="s">
         <v>390</v>
       </c>
-      <c r="T50" s="95" t="s">
+      <c r="T50" s="94" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="51" spans="1:20" s="95" customFormat="1" ht="17" x14ac:dyDescent="0.15">
-      <c r="A51" s="95">
+    <row r="51" spans="1:20" s="94" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+      <c r="A51" s="94">
         <v>41</v>
       </c>
       <c r="B51" s="38" t="s">
         <v>231</v>
       </c>
       <c r="C51" s="38"/>
-      <c r="D51" s="95" t="s">
+      <c r="D51" s="94" t="s">
         <v>392</v>
       </c>
-      <c r="E51" s="97">
+      <c r="E51" s="96">
         <v>1</v>
       </c>
       <c r="F51" s="38" t="s">
         <v>200</v>
       </c>
-      <c r="G51" s="95" t="s">
+      <c r="G51" s="94" t="s">
         <v>393</v>
       </c>
       <c r="H51" s="38" t="s">
         <v>394</v>
       </c>
-      <c r="I51" s="95" t="s">
+      <c r="I51" s="94" t="s">
         <v>219</v>
       </c>
-      <c r="J51" s="95">
+      <c r="J51" s="94">
         <v>1</v>
       </c>
       <c r="K51" s="38">
-        <f>IF(J51&gt;E51,0,E51-J51)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L51" s="38">
-        <f>J51+K51</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="M51" s="38">
-        <f>L51-E51</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N51" s="38">
-        <f>(4*E51)-M51</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="O51" s="38"/>
       <c r="P51" s="38"/>
       <c r="Q51" s="38"/>
       <c r="R51" s="38"/>
-      <c r="S51" s="95" t="s">
+      <c r="S51" s="94" t="s">
         <v>395</v>
       </c>
-      <c r="T51" s="95" t="s">
+      <c r="T51" s="94" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="52" spans="1:20" s="95" customFormat="1" ht="17" x14ac:dyDescent="0.15">
-      <c r="A52" s="95">
+    <row r="52" spans="1:20" s="94" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+      <c r="A52" s="94">
         <v>42</v>
       </c>
       <c r="B52" s="38" t="s">
         <v>396</v>
       </c>
       <c r="C52" s="38"/>
-      <c r="D52" s="95" t="s">
+      <c r="D52" s="94" t="s">
         <v>397</v>
       </c>
-      <c r="E52" s="97">
+      <c r="E52" s="96">
         <v>1</v>
       </c>
       <c r="F52" s="38" t="s">
         <v>200</v>
       </c>
-      <c r="G52" s="95" t="s">
+      <c r="G52" s="94" t="s">
         <v>398</v>
       </c>
-      <c r="H52" s="95" t="s">
+      <c r="H52" s="94" t="s">
         <v>399</v>
       </c>
-      <c r="I52" s="95" t="s">
+      <c r="I52" s="94" t="s">
         <v>219</v>
       </c>
-      <c r="J52" s="95">
+      <c r="J52" s="94">
         <v>1</v>
       </c>
       <c r="K52" s="38">
-        <f>IF(J52&gt;E52,0,E52-J52)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L52" s="38">
-        <f>J52+K52</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="M52" s="38">
-        <f>L52-E52</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N52" s="38">
-        <f>(4*E52)-M52</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="O52" s="38"/>
       <c r="P52" s="38"/>
       <c r="Q52" s="38"/>
       <c r="R52" s="38"/>
-      <c r="S52" s="95" t="s">
+      <c r="S52" s="94" t="s">
         <v>400</v>
       </c>
-      <c r="T52" s="95" t="s">
+      <c r="T52" s="94" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="53" spans="1:20" s="95" customFormat="1" ht="17" x14ac:dyDescent="0.15">
-      <c r="A53" s="95">
+    <row r="53" spans="1:20" s="94" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+      <c r="A53" s="94">
         <v>43</v>
       </c>
       <c r="B53" s="38" t="s">
         <v>401</v>
       </c>
       <c r="C53" s="38"/>
-      <c r="D53" s="95" t="s">
+      <c r="D53" s="94" t="s">
         <v>402</v>
       </c>
-      <c r="E53" s="97">
+      <c r="E53" s="96">
         <v>1</v>
       </c>
       <c r="F53" s="38" t="s">
         <v>200</v>
       </c>
-      <c r="G53" s="95" t="s">
+      <c r="G53" s="94" t="s">
         <v>403</v>
       </c>
-      <c r="I53" s="95" t="s">
+      <c r="I53" s="94" t="s">
         <v>219</v>
       </c>
-      <c r="J53" s="95">
+      <c r="J53" s="94">
         <v>1</v>
       </c>
       <c r="K53" s="38">
-        <f>IF(J53&gt;E53,0,E53-J53)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L53" s="38">
-        <f>J53+K53</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="M53" s="38">
-        <f>L53-E53</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N53" s="38">
-        <f>(4*E53)-M53</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="O53" s="38"/>
       <c r="P53" s="38"/>
       <c r="Q53" s="38"/>
       <c r="R53" s="38"/>
-      <c r="S53" s="95" t="s">
+      <c r="S53" s="94" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="54" spans="1:20" s="95" customFormat="1" ht="17" x14ac:dyDescent="0.15">
-      <c r="A54" s="95">
+    <row r="54" spans="1:20" s="94" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+      <c r="A54" s="94">
         <v>102</v>
       </c>
       <c r="B54" s="38" t="s">
         <v>260</v>
       </c>
       <c r="C54" s="38"/>
-      <c r="D54" s="95" t="s">
+      <c r="D54" s="94" t="s">
         <v>261</v>
       </c>
-      <c r="E54" s="97">
+      <c r="E54" s="96">
         <v>2</v>
       </c>
       <c r="F54" s="38" t="s">
         <v>200</v>
       </c>
-      <c r="G54" s="95" t="s">
+      <c r="G54" s="94" t="s">
         <v>407</v>
       </c>
       <c r="H54" s="38" t="s">
         <v>408</v>
       </c>
-      <c r="I54" s="95" t="s">
+      <c r="I54" s="94" t="s">
         <v>219</v>
       </c>
-      <c r="J54" s="95">
+      <c r="J54" s="94">
         <v>0</v>
       </c>
       <c r="K54" s="38">
-        <f>IF(J54&gt;E54,0,E54-J54)</f>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="L54" s="38">
-        <f>J54+K54</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="M54" s="38">
-        <f>L54-E54</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N54" s="38">
-        <f>(4*E54)-M54</f>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="O54" s="38"/>
@@ -8740,15 +8762,15 @@
       <c r="Q54" s="38"/>
       <c r="R54" s="38"/>
     </row>
-    <row r="55" spans="1:20" s="95" customFormat="1" ht="17" x14ac:dyDescent="0.15">
-      <c r="A55" s="95">
+    <row r="55" spans="1:20" s="94" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+      <c r="A55" s="94">
         <v>105</v>
       </c>
-      <c r="B55" s="95" t="s">
+      <c r="B55" s="94" t="s">
         <v>142</v>
       </c>
       <c r="D55" s="38"/>
-      <c r="E55" s="97">
+      <c r="E55" s="96">
         <v>1</v>
       </c>
       <c r="F55" s="38" t="s">
@@ -8758,26 +8780,26 @@
       <c r="H55" s="38" t="s">
         <v>409</v>
       </c>
-      <c r="I55" s="95" t="s">
+      <c r="I55" s="94" t="s">
         <v>203</v>
       </c>
-      <c r="J55" s="95">
+      <c r="J55" s="94">
         <v>5</v>
       </c>
-      <c r="K55" s="95">
-        <f>IF(J55&gt;E55,0,E55-J55)</f>
-        <v>0</v>
-      </c>
-      <c r="L55" s="95">
-        <f>J55+K55</f>
+      <c r="K55" s="94">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="L55" s="94">
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="M55" s="95">
-        <f>L55-E55</f>
+      <c r="M55" s="94">
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
-      <c r="N55" s="95">
-        <f>(4*E55)-M55</f>
+      <c r="N55" s="94">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="P55" s="38"/>
@@ -8905,7 +8927,7 @@
   <mergeCells count="1">
     <mergeCell ref="P7:R7"/>
   </mergeCells>
-  <phoneticPr fontId="18" type="noConversion"/>
+  <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -8947,11 +8969,11 @@
       <c r="A3" s="29"/>
       <c r="B3" s="27"/>
       <c r="C3" s="27"/>
-      <c r="P3" s="86" t="s">
+      <c r="P3" s="99" t="s">
         <v>173</v>
       </c>
-      <c r="Q3" s="86"/>
-      <c r="R3" s="86"/>
+      <c r="Q3" s="99"/>
+      <c r="R3" s="99"/>
     </row>
     <row r="4" spans="1:18" ht="17" x14ac:dyDescent="0.15">
       <c r="A4" s="29"/>
@@ -9409,7 +9431,7 @@
     </row>
     <row r="24" spans="1:20" s="38" customFormat="1" ht="24" x14ac:dyDescent="0.15">
       <c r="A24" s="66"/>
-      <c r="B24" s="94" t="s">
+      <c r="B24" s="93" t="s">
         <v>538</v>
       </c>
       <c r="D24" s="67"/>
@@ -9420,19 +9442,19 @@
     </row>
     <row r="25" spans="1:20" s="73" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="B25" s="30"/>
-      <c r="C25" s="92" t="s">
+      <c r="C25" s="91" t="s">
         <v>500</v>
       </c>
       <c r="E25" s="74">
         <v>1</v>
       </c>
-      <c r="F25" s="91" t="s">
+      <c r="F25" s="90" t="s">
         <v>200</v>
       </c>
-      <c r="G25" s="92" t="s">
+      <c r="G25" s="91" t="s">
         <v>517</v>
       </c>
-      <c r="H25" s="92" t="s">
+      <c r="H25" s="91" t="s">
         <v>516</v>
       </c>
       <c r="J25" s="73">
@@ -9466,22 +9488,22 @@
     </row>
     <row r="26" spans="1:20" s="73" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="B26" s="30"/>
-      <c r="C26" s="90" t="s">
+      <c r="C26" s="89" t="s">
         <v>532</v>
       </c>
-      <c r="D26" s="90" t="s">
+      <c r="D26" s="89" t="s">
         <v>531</v>
       </c>
       <c r="E26" s="74">
         <v>2</v>
       </c>
-      <c r="F26" s="91" t="s">
+      <c r="F26" s="90" t="s">
         <v>200</v>
       </c>
-      <c r="G26" s="92" t="s">
+      <c r="G26" s="91" t="s">
         <v>515</v>
       </c>
-      <c r="H26" s="92" t="s">
+      <c r="H26" s="91" t="s">
         <v>514</v>
       </c>
       <c r="J26" s="73">
@@ -9503,22 +9525,22 @@
     </row>
     <row r="27" spans="1:20" s="73" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="B27" s="30"/>
-      <c r="C27" s="92" t="s">
+      <c r="C27" s="91" t="s">
         <v>511</v>
       </c>
-      <c r="D27" s="92" t="s">
+      <c r="D27" s="91" t="s">
         <v>513</v>
       </c>
       <c r="E27" s="74">
         <v>1</v>
       </c>
-      <c r="F27" s="91" t="s">
+      <c r="F27" s="90" t="s">
         <v>200</v>
       </c>
-      <c r="G27" s="92" t="s">
+      <c r="G27" s="91" t="s">
         <v>512</v>
       </c>
-      <c r="H27" s="92" t="s">
+      <c r="H27" s="91" t="s">
         <v>510</v>
       </c>
       <c r="J27" s="73">
@@ -9538,16 +9560,16 @@
       <c r="Q27" s="30"/>
       <c r="R27" s="30"/>
     </row>
-    <row r="28" spans="1:20" s="95" customFormat="1" ht="21" x14ac:dyDescent="0.15">
-      <c r="B28" s="94" t="s">
+    <row r="28" spans="1:20" s="94" customFormat="1" ht="21" x14ac:dyDescent="0.15">
+      <c r="B28" s="93" t="s">
         <v>539</v>
       </c>
-      <c r="C28" s="96"/>
-      <c r="D28" s="96"/>
-      <c r="E28" s="97"/>
+      <c r="C28" s="95"/>
+      <c r="D28" s="95"/>
+      <c r="E28" s="96"/>
       <c r="F28" s="65"/>
-      <c r="G28" s="96"/>
-      <c r="H28" s="96"/>
+      <c r="G28" s="95"/>
+      <c r="H28" s="95"/>
       <c r="K28" s="38"/>
       <c r="M28" s="38"/>
       <c r="N28" s="38"/>
@@ -9556,7 +9578,7 @@
       <c r="Q28" s="38"/>
       <c r="R28" s="38"/>
     </row>
-    <row r="29" spans="1:20" s="27" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:20" s="27" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="B29" s="77"/>
       <c r="C29" s="77"/>
       <c r="D29" s="78" t="s">
@@ -9574,16 +9596,16 @@
       <c r="Q29" s="28"/>
       <c r="R29" s="28"/>
     </row>
-    <row r="30" spans="1:20" s="95" customFormat="1" ht="21" x14ac:dyDescent="0.15">
-      <c r="B30" s="94" t="s">
+    <row r="30" spans="1:20" s="94" customFormat="1" ht="21" x14ac:dyDescent="0.15">
+      <c r="B30" s="93" t="s">
         <v>540</v>
       </c>
-      <c r="C30" s="96"/>
-      <c r="D30" s="96"/>
-      <c r="E30" s="97"/>
+      <c r="C30" s="95"/>
+      <c r="D30" s="95"/>
+      <c r="E30" s="96"/>
       <c r="F30" s="65"/>
-      <c r="G30" s="96"/>
-      <c r="H30" s="96"/>
+      <c r="G30" s="95"/>
+      <c r="H30" s="95"/>
       <c r="K30" s="38"/>
       <c r="M30" s="38"/>
       <c r="N30" s="38"/>
@@ -9604,16 +9626,16 @@
       <c r="Q31" s="28"/>
       <c r="R31" s="28"/>
     </row>
-    <row r="32" spans="1:20" s="95" customFormat="1" ht="21" x14ac:dyDescent="0.15">
-      <c r="B32" s="94" t="s">
+    <row r="32" spans="1:20" s="94" customFormat="1" ht="21" x14ac:dyDescent="0.15">
+      <c r="B32" s="93" t="s">
         <v>541</v>
       </c>
-      <c r="C32" s="96"/>
-      <c r="D32" s="96"/>
-      <c r="E32" s="97"/>
+      <c r="C32" s="95"/>
+      <c r="D32" s="95"/>
+      <c r="E32" s="96"/>
       <c r="F32" s="65"/>
-      <c r="G32" s="96"/>
-      <c r="H32" s="96"/>
+      <c r="G32" s="95"/>
+      <c r="H32" s="95"/>
       <c r="K32" s="38"/>
       <c r="M32" s="38"/>
       <c r="N32" s="38"/>
@@ -9700,11 +9722,11 @@
       <c r="A3" s="29"/>
       <c r="B3" s="27"/>
       <c r="C3" s="27"/>
-      <c r="P3" s="86" t="s">
+      <c r="P3" s="99" t="s">
         <v>173</v>
       </c>
-      <c r="Q3" s="86"/>
-      <c r="R3" s="86"/>
+      <c r="Q3" s="99"/>
+      <c r="R3" s="99"/>
     </row>
     <row r="4" spans="1:18" ht="17" x14ac:dyDescent="0.15">
       <c r="A4" s="29"/>
@@ -9823,7 +9845,7 @@
     </row>
     <row r="8" spans="1:18" s="38" customFormat="1" ht="24" x14ac:dyDescent="0.15">
       <c r="A8" s="66"/>
-      <c r="B8" s="94" t="s">
+      <c r="B8" s="93" t="s">
         <v>535</v>
       </c>
       <c r="D8" s="67"/>
@@ -9832,22 +9854,22 @@
       <c r="I8" s="67"/>
       <c r="R8" s="39"/>
     </row>
-    <row r="9" spans="1:18" s="73" customFormat="1" ht="85" x14ac:dyDescent="0.15">
-      <c r="C9" s="93" t="s">
+    <row r="9" spans="1:18" s="73" customFormat="1" ht="102" x14ac:dyDescent="0.15">
+      <c r="C9" s="92" t="s">
         <v>533</v>
       </c>
-      <c r="D9" s="91" t="s">
+      <c r="D9" s="90" t="s">
         <v>491</v>
       </c>
       <c r="E9" s="74"/>
       <c r="F9" s="30"/>
-      <c r="G9" s="93" t="s">
+      <c r="G9" s="92" t="s">
         <v>534</v>
       </c>
-      <c r="H9" s="91" t="s">
+      <c r="H9" s="90" t="s">
         <v>492</v>
       </c>
-      <c r="I9" s="90" t="s">
+      <c r="I9" s="89" t="s">
         <v>219</v>
       </c>
       <c r="J9" s="73">
@@ -9864,13 +9886,13 @@
       <c r="R9" s="30"/>
     </row>
     <row r="10" spans="1:18" s="27" customFormat="1" ht="21" x14ac:dyDescent="0.15">
-      <c r="B10" s="94" t="s">
+      <c r="B10" s="93" t="s">
         <v>536</v>
       </c>
       <c r="E10" s="72"/>
       <c r="F10" s="28"/>
-      <c r="G10" s="88"/>
-      <c r="H10" s="88"/>
+      <c r="G10" s="87"/>
+      <c r="H10" s="87"/>
       <c r="K10" s="28"/>
       <c r="L10" s="28"/>
       <c r="M10" s="28"/>
@@ -9957,19 +9979,19 @@
       <c r="R14" s="28"/>
     </row>
     <row r="15" spans="1:18" s="27" customFormat="1" ht="21" x14ac:dyDescent="0.15">
-      <c r="B15" s="94" t="s">
+      <c r="B15" s="93" t="s">
         <v>536</v>
       </c>
       <c r="D15" s="28"/>
       <c r="E15" s="72"/>
       <c r="F15" s="28"/>
       <c r="G15" s="28"/>
-      <c r="H15" s="89"/>
+      <c r="H15" s="88"/>
       <c r="P15" s="28"/>
       <c r="Q15" s="28"/>
       <c r="R15" s="28"/>
     </row>
-    <row r="16" spans="1:18" s="80" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:18" s="80" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="C16" s="81" t="s">
         <v>506</v>
       </c>
@@ -10001,13 +10023,13 @@
       <c r="Q16" s="54"/>
       <c r="R16" s="54"/>
     </row>
-    <row r="17" spans="2:18" s="95" customFormat="1" ht="21" x14ac:dyDescent="0.15">
-      <c r="B17" s="94" t="s">
+    <row r="17" spans="2:18" s="94" customFormat="1" ht="21" x14ac:dyDescent="0.15">
+      <c r="B17" s="93" t="s">
         <v>537</v>
       </c>
-      <c r="C17" s="96"/>
+      <c r="C17" s="95"/>
       <c r="D17" s="65"/>
-      <c r="E17" s="97"/>
+      <c r="E17" s="96"/>
       <c r="F17" s="65"/>
       <c r="G17" s="65"/>
       <c r="H17" s="65"/>
@@ -10017,14 +10039,14 @@
     </row>
     <row r="18" spans="2:18" s="27" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="B18" s="82"/>
-      <c r="C18" s="88" t="s">
+      <c r="C18" s="87" t="s">
         <v>528</v>
       </c>
       <c r="D18" s="28"/>
       <c r="E18" s="72">
         <v>1</v>
       </c>
-      <c r="F18" s="89" t="s">
+      <c r="F18" s="88" t="s">
         <v>200</v>
       </c>
       <c r="G18" s="27" t="s">
@@ -10068,12 +10090,12 @@
       <c r="E19" s="27">
         <v>1</v>
       </c>
-      <c r="F19" s="89" t="s">
+      <c r="F19" s="88" t="s">
         <v>200</v>
       </c>
       <c r="G19" s="28"/>
       <c r="H19" s="28"/>
-      <c r="I19" s="88" t="s">
+      <c r="I19" s="87" t="s">
         <v>219</v>
       </c>
       <c r="J19" s="27">
@@ -10091,12 +10113,12 @@
       <c r="E20" s="27">
         <v>1</v>
       </c>
-      <c r="F20" s="89" t="s">
+      <c r="F20" s="88" t="s">
         <v>200</v>
       </c>
       <c r="G20" s="28"/>
       <c r="H20" s="28"/>
-      <c r="I20" s="88" t="s">
+      <c r="I20" s="87" t="s">
         <v>219</v>
       </c>
       <c r="J20" s="27">
@@ -10114,12 +10136,12 @@
       <c r="E21" s="27">
         <v>1</v>
       </c>
-      <c r="F21" s="89" t="s">
+      <c r="F21" s="88" t="s">
         <v>200</v>
       </c>
       <c r="G21" s="28"/>
       <c r="H21" s="28"/>
-      <c r="I21" s="88" t="s">
+      <c r="I21" s="87" t="s">
         <v>219</v>
       </c>
       <c r="J21" s="27">
@@ -10130,7 +10152,7 @@
       <c r="R21" s="28"/>
     </row>
     <row r="22" spans="2:18" s="27" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="C22" s="88" t="s">
+      <c r="C22" s="87" t="s">
         <v>529</v>
       </c>
       <c r="D22" s="28"/>
@@ -10142,7 +10164,7 @@
       <c r="R22" s="28"/>
     </row>
     <row r="23" spans="2:18" s="27" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="C23" s="88" t="s">
+      <c r="C23" s="87" t="s">
         <v>530</v>
       </c>
       <c r="D23" s="28"/>
@@ -10155,7 +10177,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A6:N6" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:N6">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:N7">
       <sortCondition ref="B6"/>
     </sortState>
   </autoFilter>

</xml_diff>